<commit_message>
re-add cluster 1 data
</commit_message>
<xml_diff>
--- a/scrapers/clusters/Clusters-Sumulas.xlsx
+++ b/scrapers/clusters/Clusters-Sumulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silla\Desktop\Projetos\-sailing-rankings-2024.1\scrapers\clusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE5F7A-ED18-4925-80E8-2943FA1DEC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E9742B-01D7-4B25-B369-A4F03ED5CC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTROLE" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="501">
   <si>
     <t>TAREFA</t>
   </si>
@@ -2186,11 +2186,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2627,9 +2627,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>49530</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7010400" cy="3333750"/>
     <xdr:pic>
@@ -2650,6 +2650,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6198870" y="182880"/>
+          <a:ext cx="7010400" cy="3333750"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -3100,10 +3104,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -3119,8 +3123,8 @@
       <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
@@ -12301,7 +12305,7 @@
   </sheetPr>
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -12330,7 +12334,7 @@
       <c r="E1" s="44" t="s">
         <v>421</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="72" t="s">
         <v>500</v>
       </c>
     </row>
@@ -12358,7 +12362,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="13.2">
       <c r="A3" s="45" t="s">
         <v>42</v>
       </c>
@@ -12400,7 +12404,7 @@
         <v>Semaine Olympique Francaise De Voile 2023</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="13.2">
       <c r="A5" s="45" t="s">
         <v>147</v>
       </c>
@@ -12442,7 +12446,7 @@
         <v>Semaine Olympique Francaise De Voile 2023</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="13.2">
       <c r="A7" s="45" t="s">
         <v>225</v>
       </c>
@@ -12463,7 +12467,7 @@
         <v>World Championship 2022</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="13.2">
       <c r="A8" s="45" t="s">
         <v>201</v>
       </c>
@@ -12484,7 +12488,7 @@
         <v>World Championship 2022</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="13.2">
       <c r="A9" s="45" t="s">
         <v>201</v>
       </c>
@@ -12505,7 +12509,7 @@
         <v>European Championship 2022</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="13.2">
       <c r="A10" s="45" t="s">
         <v>436</v>
       </c>
@@ -12526,7 +12530,7 @@
         <v>European Championship 2022</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="13.2">
       <c r="A11" s="45" t="s">
         <v>201</v>
       </c>
@@ -12547,7 +12551,7 @@
         <v>European Championship 2023</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="13.2">
       <c r="A12" s="45" t="s">
         <v>225</v>
       </c>
@@ -12568,7 +12572,7 @@
         <v>European Championship 2023</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="13.2">
       <c r="A13" s="45" t="s">
         <v>225</v>
       </c>
@@ -12589,7 +12593,7 @@
         <v>Trofeo S.A.R Princesa Sofia 2023</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="13.2">
       <c r="A14" s="45" t="s">
         <v>201</v>
       </c>
@@ -12697,7 +12701,7 @@
         <v>Semaine Olympique Francaise De Voile 2023</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="13.2">
       <c r="A19" s="45" t="s">
         <v>243</v>
       </c>
@@ -12718,7 +12722,7 @@
         <v>Trofeo S.A.R Princesa Sofia 2023</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="13.2">
       <c r="A20" s="45" t="s">
         <v>311</v>
       </c>
@@ -12823,7 +12827,7 @@
         <v>Semaine Olympique Francaise De Voile 2023</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="13.2">
       <c r="A25" s="45">
         <v>470</v>
       </c>
@@ -12844,7 +12848,7 @@
         <v>World Championship 2022</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="13.2">
       <c r="A26" s="45">
         <v>470</v>
       </c>
@@ -12865,7 +12869,7 @@
         <v>European Championship 2022</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="13.2">
       <c r="A27" s="45">
         <v>470</v>
       </c>
@@ -16995,7 +16999,9 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -17382,7 +17388,9 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -17496,7 +17504,9 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -17505,6 +17515,7 @@
     <col min="3" max="3" width="6.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -17523,6 +17534,9 @@
       <c r="E1" s="44" t="s">
         <v>421</v>
       </c>
+      <c r="F1" s="44" t="s">
+        <v>500</v>
+      </c>
       <c r="G1" s="2" t="s">
         <v>476</v>
       </c>
@@ -17543,6 +17557,10 @@
       <c r="E2" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(B2," ",C2)</f>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="45" t="s">
@@ -17560,6 +17578,10 @@
       <c r="E3" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F11" si="0">_xlfn.CONCAT(B3," ",C3)</f>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="45" t="s">
@@ -17577,6 +17599,10 @@
       <c r="E4" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="45" t="s">
@@ -17594,6 +17620,10 @@
       <c r="E5" s="27" t="s">
         <v>455</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="45" t="s">
@@ -17611,6 +17641,10 @@
       <c r="E6" s="27" t="s">
         <v>455</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="45" t="s">
@@ -17628,6 +17662,10 @@
       <c r="E7" s="27" t="s">
         <v>455</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="45">
@@ -17645,6 +17683,10 @@
       <c r="E8" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="45" t="s">
@@ -17662,6 +17704,10 @@
       <c r="E9" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="63" t="s">
@@ -17679,6 +17725,10 @@
       <c r="E10" s="2" t="s">
         <v>455</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="63" t="s">
@@ -17695,6 +17745,10 @@
       </c>
       <c r="E11" s="2" t="s">
         <v>455</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>World Championship 2023</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -20777,7 +20831,7 @@
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13.2">
       <c r="A1" s="43" t="s">
         <v>417</v>
       </c>
@@ -20865,73 +20919,73 @@
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="13.2">
       <c r="A6" s="58"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="13.2">
       <c r="A7" s="58"/>
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="13.2">
       <c r="A8" s="58"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="13.2">
       <c r="A9" s="58"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="13.2">
       <c r="A10" s="58"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="13.2">
       <c r="A11" s="58"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="13.2">
       <c r="A12" s="58"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="13.2">
       <c r="A13" s="58"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="13.2">
       <c r="A14" s="58"/>
       <c r="E14" s="27"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="13.2">
       <c r="A15" s="58"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="13.2">
       <c r="A16" s="58"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" ht="13.2">
       <c r="A17" s="58"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" ht="13.2">
       <c r="A18" s="58"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" ht="13.2">
       <c r="A19" s="58"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" ht="13.2">
       <c r="A20" s="58"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" ht="13.2">
       <c r="A21" s="58"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" ht="13.2">
       <c r="A22" s="58"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" ht="13.2">
       <c r="A23" s="58"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" ht="13.2">
       <c r="A24" s="58"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" ht="13.2">
       <c r="A25" s="58"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" ht="13.2">
       <c r="A26" s="58"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="13.2">
       <c r="A27" s="58"/>
     </row>
     <row r="28" spans="1:1" ht="13.2">

</xml_diff>

<commit_message>
add cluster 3 data e kite mas e fem
</commit_message>
<xml_diff>
--- a/scrapers/clusters/Clusters-Sumulas.xlsx
+++ b/scrapers/clusters/Clusters-Sumulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silla\Desktop\Projetos\-sailing-rankings-2024.1\scrapers\clusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E9742B-01D7-4B25-B369-A4F03ED5CC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD44AF6-F5B6-4BB0-9579-8BC12DAA8C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTROLE" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="511">
   <si>
     <t>TAREFA</t>
   </si>
@@ -1644,6 +1644,36 @@
   </si>
   <si>
     <t>Competição</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/e3a84d68-a53c-41a1-857a-8ffa30834afa?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/3857831a-a7f8-4203-a0be-c1fa9675fa36?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/1717a706-5422-406a-861a-e8d23c2f5ede?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/f28441e7-4b5a-4b28-aa66-0c6a90c99554?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/b04bd77a-378c-4737-85c6-3a740b95cdcb?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/0d045360-396f-47f8-98ab-baf443431020?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/1eed37b0-cdb7-4676-9489-599016df98ef?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/264ee773-4617-402e-ab62-c666386ddf0b?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/7498c006-6590-44fd-97b7-654df8e76cd9?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/938dd1e3-0b3d-437d-9790-1081538fbcd4?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
   </si>
 </sst>
 </file>
@@ -12305,7 +12335,7 @@
   </sheetPr>
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -17000,7 +17030,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -17389,7 +17419,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -17505,7 +17535,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -17552,7 +17582,7 @@
         <v>2023</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>44</v>
+        <v>503</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>455</v>
@@ -17573,7 +17603,7 @@
         <v>2023</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>44</v>
+        <v>504</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>455</v>
@@ -17594,7 +17624,7 @@
         <v>2023</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>44</v>
+        <v>501</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>455</v>
@@ -17615,7 +17645,7 @@
         <v>2023</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>44</v>
+        <v>502</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>455</v>
@@ -17636,7 +17666,7 @@
         <v>2023</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>44</v>
+        <v>507</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>455</v>
@@ -17657,7 +17687,7 @@
         <v>2023</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>44</v>
+        <v>506</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>455</v>
@@ -17678,7 +17708,7 @@
         <v>2023</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>44</v>
+        <v>505</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>455</v>
@@ -17699,7 +17729,7 @@
         <v>2023</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>44</v>
+        <v>508</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>455</v>
@@ -17720,7 +17750,7 @@
         <v>2023</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>44</v>
+        <v>509</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>455</v>
@@ -17741,7 +17771,7 @@
         <v>2023</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>44</v>
+        <v>510</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>455</v>
@@ -20719,20 +20749,8 @@
       <c r="A1000" s="58"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add cluster 14 data
</commit_message>
<xml_diff>
--- a/scrapers/clusters/Clusters-Sumulas.xlsx
+++ b/scrapers/clusters/Clusters-Sumulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silla\Desktop\Projetos\-sailing-rankings-2024.1\scrapers\clusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD44AF6-F5B6-4BB0-9579-8BC12DAA8C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34754EF1-0E90-4EF1-AE45-D8AA297230B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTROLE" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Cluster 11" sheetId="14" r:id="rId14"/>
     <sheet name="Cluster 12" sheetId="15" r:id="rId15"/>
     <sheet name="Cluster 13" sheetId="16" r:id="rId16"/>
+    <sheet name="Cluster 14" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="531">
   <si>
     <t>TAREFA</t>
   </si>
@@ -1675,12 +1676,72 @@
   <si>
     <t>https://world-sailing-api.soticcloud.net/stats/api/event/938dd1e3-0b3d-437d-9790-1081538fbcd4?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins</t>
   </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/5723bc4c-e856-45d0-b72d-6d2ef4555b58?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/d85dd4e5-9367-4c1c-9008-fe351b02dbde?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/dcc8e735-0af4-4dc4-ae9b-078f5ceb3088?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/b053edb1-8e2e-4335-9901-2c2db3e046bb?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/76d820c6-7055-4da1-88d4-da95bb145b2a?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/8168190c-71cb-4aba-a585-83faec4d4c75?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/2f8c782d-70fc-4740-bfd6-f0d4ba07a29f?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/7714c998-8785-40bd-b8f2-1d01782f4f25?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/7a9738ba-34be-4150-9de0-cc4e8f289f90?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/93af2e7f-a9c9-4a0a-adac-eeb0e8ef5ae8?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/37962828-6446-4771-82be-da80dad137fe?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/258965db-91d5-41dd-9883-d465f1afc95b?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/25f4338b-2517-4f28-beef-c980a8fb906d?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/4eee496c-8981-4247-bcf9-b11eb6cdff08?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/8e8d45fc-7f9e-4ce5-8931-9cfe44430ace?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/947c88bb-efad-409b-92bf-33d4b4447895?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/a1e9c72b-c078-434f-9978-784bd8a8c864?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/b4da1710-1db1-4d82-bb1c-e59c06e3ec2b?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/c4a77e1c-0c76-4e1b-bb67-b17aa0fd9c05?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
+  <si>
+    <t>https://world-sailing-api.soticcloud.net/stats/api/event/da3db27d-3219-4398-bd3d-95fef026ac3c?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="42">
+  <fonts count="45">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1933,6 +1994,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -2074,10 +2156,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2217,12 +2300,19 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3134,10 +3224,10 @@
         <v>7</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="74"/>
+      <c r="H2" s="78"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -3153,8 +3243,8 @@
       <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
@@ -3401,7 +3491,9 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -3958,6 +4050,409 @@
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633AD511-4328-4D4D-A2DB-A7C59751CCA8}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="43" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>421</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C2">
+        <v>2015</v>
+      </c>
+      <c r="D2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(B2," ",C2)</f>
+        <v>Semaine Olympique Francaise De Voile 2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C3">
+        <v>2015</v>
+      </c>
+      <c r="D3" t="s">
+        <v>512</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT(B3," ",C3)</f>
+        <v>Semaine Olympique Francaise De Voile 2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>428</v>
+      </c>
+      <c r="C4">
+        <v>2015</v>
+      </c>
+      <c r="D4" t="s">
+        <v>513</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT(B4," ",C4)</f>
+        <v>Semaine Olympique Francaise De Voile 2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="58" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C5">
+        <v>2015</v>
+      </c>
+      <c r="D5" t="s">
+        <v>514</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F21" si="0">_xlfn.CONCAT(B5," ",C5)</f>
+        <v>Semaine Olympique Francaise De Voile 2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="75" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6" s="73" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6">
+        <v>2015</v>
+      </c>
+      <c r="D6" t="s">
+        <v>515</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C7">
+        <v>2016</v>
+      </c>
+      <c r="D7" t="s">
+        <v>516</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C8">
+        <v>2016</v>
+      </c>
+      <c r="D8" t="s">
+        <v>517</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" t="s">
+        <v>428</v>
+      </c>
+      <c r="C9">
+        <v>2016</v>
+      </c>
+      <c r="D9" t="s">
+        <v>518</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="58" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" t="s">
+        <v>428</v>
+      </c>
+      <c r="C10">
+        <v>2016</v>
+      </c>
+      <c r="D10" t="s">
+        <v>519</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="75" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>428</v>
+      </c>
+      <c r="C11">
+        <v>2016</v>
+      </c>
+      <c r="D11" t="s">
+        <v>520</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>428</v>
+      </c>
+      <c r="C12">
+        <v>2023</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>521</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>428</v>
+      </c>
+      <c r="C13">
+        <v>2023</v>
+      </c>
+      <c r="D13" t="s">
+        <v>525</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" t="s">
+        <v>428</v>
+      </c>
+      <c r="C14">
+        <v>2023</v>
+      </c>
+      <c r="D14" t="s">
+        <v>523</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="58" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" t="s">
+        <v>428</v>
+      </c>
+      <c r="C15">
+        <v>2023</v>
+      </c>
+      <c r="D15" t="s">
+        <v>526</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="75" t="s">
+        <v>361</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>428</v>
+      </c>
+      <c r="C16">
+        <v>2023</v>
+      </c>
+      <c r="D16" t="s">
+        <v>522</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>470</v>
+      </c>
+      <c r="B17" t="s">
+        <v>428</v>
+      </c>
+      <c r="C17">
+        <v>2023</v>
+      </c>
+      <c r="D17" t="s">
+        <v>527</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B18" t="s">
+        <v>428</v>
+      </c>
+      <c r="C18">
+        <v>2023</v>
+      </c>
+      <c r="D18" t="s">
+        <v>524</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B19" t="s">
+        <v>428</v>
+      </c>
+      <c r="C19">
+        <v>2023</v>
+      </c>
+      <c r="D19" t="s">
+        <v>530</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>436</v>
+      </c>
+      <c r="B20" t="s">
+        <v>428</v>
+      </c>
+      <c r="C20">
+        <v>2023</v>
+      </c>
+      <c r="D20" t="s">
+        <v>528</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="73" t="s">
+        <v>428</v>
+      </c>
+      <c r="C21">
+        <v>2023</v>
+      </c>
+      <c r="D21" t="s">
+        <v>529</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>Semaine Olympique Francaise De Voile 2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1" display="https://world-sailing-api.soticcloud.net/stats/api/event/37962828-6446-4771-82be-da80dad137fe?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status" xr:uid="{510C4EAC-39B3-42B6-9B2A-5456F66BE504}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -12335,8 +12830,8 @@
   </sheetPr>
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -17534,21 +18029,21 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="13.2">
       <c r="A1" s="43" t="s">
         <v>417</v>
       </c>
@@ -17571,7 +18066,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="13.2">
       <c r="A2" s="45" t="s">
         <v>42</v>
       </c>
@@ -17592,7 +18087,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="13.2">
       <c r="A3" s="45" t="s">
         <v>147</v>
       </c>
@@ -17613,7 +18108,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="13.2">
       <c r="A4" s="45" t="s">
         <v>436</v>
       </c>
@@ -17634,7 +18129,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="13.2">
       <c r="A5" s="45" t="s">
         <v>201</v>
       </c>
@@ -17655,7 +18150,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="13.2">
       <c r="A6" s="45" t="s">
         <v>311</v>
       </c>
@@ -17676,7 +18171,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="13.2">
       <c r="A7" s="45" t="s">
         <v>243</v>
       </c>
@@ -17697,7 +18192,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="13.2">
       <c r="A8" s="45">
         <v>470</v>
       </c>
@@ -17707,7 +18202,7 @@
       <c r="C8" s="3">
         <v>2023</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="74" t="s">
         <v>505</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -17718,7 +18213,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="13.2">
       <c r="A9" s="45" t="s">
         <v>361</v>
       </c>
@@ -17739,7 +18234,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="13.2">
       <c r="A10" s="63" t="s">
         <v>389</v>
       </c>
@@ -17760,7 +18255,7 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="13.2">
       <c r="A11" s="63" t="s">
         <v>405</v>
       </c>
@@ -17781,2976 +18276,2953 @@
         <v>World Championship 2023</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="58"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="58"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="58"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="58"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="58"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="58"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="58"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="58"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="58"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="58"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="58"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="58"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="58"/>
-    </row>
-    <row r="25" spans="1:1">
+    <row r="12" spans="1:7" ht="13.2"/>
+    <row r="13" spans="1:7" ht="13.2"/>
+    <row r="14" spans="1:7" ht="13.2"/>
+    <row r="15" spans="1:7" ht="13.2"/>
+    <row r="16" spans="1:7" ht="13.2"/>
+    <row r="17" spans="1:1" ht="13.2"/>
+    <row r="18" spans="1:1" ht="13.2"/>
+    <row r="19" spans="1:1" ht="13.2"/>
+    <row r="20" spans="1:1" ht="13.2"/>
+    <row r="21" spans="1:1" ht="13.2"/>
+    <row r="22" spans="1:1" ht="13.2"/>
+    <row r="23" spans="1:1" ht="13.2"/>
+    <row r="24" spans="1:1" ht="13.2"/>
+    <row r="25" spans="1:1" ht="13.2">
       <c r="A25" s="58"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" ht="13.2">
       <c r="A26" s="58"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="13.2">
       <c r="A27" s="58"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" ht="13.2">
       <c r="A28" s="58"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" ht="13.2">
       <c r="A29" s="58"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" ht="13.2">
       <c r="A30" s="58"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" ht="13.2">
       <c r="A31" s="58"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" ht="13.2">
       <c r="A32" s="58"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" ht="13.2">
       <c r="A33" s="58"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" ht="13.2">
       <c r="A34" s="58"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" ht="13.2">
       <c r="A35" s="58"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" ht="13.2">
       <c r="A36" s="58"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" ht="13.2">
       <c r="A37" s="58"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" ht="13.2">
       <c r="A38" s="58"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" ht="13.2">
       <c r="A39" s="58"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" ht="13.2">
       <c r="A40" s="58"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" ht="13.2">
       <c r="A41" s="58"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" ht="13.2">
       <c r="A42" s="58"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" ht="13.2">
       <c r="A43" s="58"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" ht="13.2">
       <c r="A44" s="58"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" ht="13.2">
       <c r="A45" s="58"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" ht="13.2">
       <c r="A46" s="58"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" ht="13.2">
       <c r="A47" s="58"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" ht="13.2">
       <c r="A48" s="58"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" ht="13.2">
       <c r="A49" s="58"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" ht="13.2">
       <c r="A50" s="58"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" ht="13.2">
       <c r="A51" s="58"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" ht="13.2">
       <c r="A52" s="58"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" ht="13.2">
       <c r="A53" s="58"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" ht="13.2">
       <c r="A54" s="58"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" ht="13.2">
       <c r="A55" s="58"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" ht="13.2">
       <c r="A56" s="58"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" ht="13.2">
       <c r="A57" s="58"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" ht="13.2">
       <c r="A58" s="58"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" ht="13.2">
       <c r="A59" s="58"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" ht="13.2">
       <c r="A60" s="58"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" ht="13.2">
       <c r="A61" s="58"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" ht="13.2">
       <c r="A62" s="58"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" ht="13.2">
       <c r="A63" s="58"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" ht="13.2">
       <c r="A64" s="58"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" ht="13.2">
       <c r="A65" s="58"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" ht="13.2">
       <c r="A66" s="58"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" ht="13.2">
       <c r="A67" s="58"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" ht="13.2">
       <c r="A68" s="58"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" ht="13.2">
       <c r="A69" s="58"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" ht="13.2">
       <c r="A70" s="58"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" ht="13.2">
       <c r="A71" s="58"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" ht="13.2">
       <c r="A72" s="58"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" ht="13.2">
       <c r="A73" s="58"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" ht="13.2">
       <c r="A74" s="58"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" ht="13.2">
       <c r="A75" s="58"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" ht="13.2">
       <c r="A76" s="58"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" ht="13.2">
       <c r="A77" s="58"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" ht="13.2">
       <c r="A78" s="58"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" ht="13.2">
       <c r="A79" s="58"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" ht="13.2">
       <c r="A80" s="58"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" ht="13.2">
       <c r="A81" s="58"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" ht="13.2">
       <c r="A82" s="58"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" ht="13.2">
       <c r="A83" s="58"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" ht="13.2">
       <c r="A84" s="58"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" ht="13.2">
       <c r="A85" s="58"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" ht="13.2">
       <c r="A86" s="58"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" ht="13.2">
       <c r="A87" s="58"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" ht="13.2">
       <c r="A88" s="58"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" ht="13.2">
       <c r="A89" s="58"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" ht="13.2">
       <c r="A90" s="58"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" ht="13.2">
       <c r="A91" s="58"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" ht="13.2">
       <c r="A92" s="58"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" ht="13.2">
       <c r="A93" s="58"/>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" ht="13.2">
       <c r="A94" s="58"/>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" ht="13.2">
       <c r="A95" s="58"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" ht="13.2">
       <c r="A96" s="58"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" ht="13.2">
       <c r="A97" s="58"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" ht="13.2">
       <c r="A98" s="58"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" ht="13.2">
       <c r="A99" s="58"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" ht="13.2">
       <c r="A100" s="58"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" ht="13.2">
       <c r="A101" s="58"/>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" ht="13.2">
       <c r="A102" s="58"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" ht="13.2">
       <c r="A103" s="58"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" ht="13.2">
       <c r="A104" s="58"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" ht="13.2">
       <c r="A105" s="58"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" ht="13.2">
       <c r="A106" s="58"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" ht="13.2">
       <c r="A107" s="58"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" ht="13.2">
       <c r="A108" s="58"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" ht="13.2">
       <c r="A109" s="58"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" ht="13.2">
       <c r="A110" s="58"/>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" ht="13.2">
       <c r="A111" s="58"/>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" ht="13.2">
       <c r="A112" s="58"/>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" ht="13.2">
       <c r="A113" s="58"/>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" ht="13.2">
       <c r="A114" s="58"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" ht="13.2">
       <c r="A115" s="58"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" ht="13.2">
       <c r="A116" s="58"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" ht="13.2">
       <c r="A117" s="58"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" ht="13.2">
       <c r="A118" s="58"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" ht="13.2">
       <c r="A119" s="58"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" ht="13.2">
       <c r="A120" s="58"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" ht="13.2">
       <c r="A121" s="58"/>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" ht="13.2">
       <c r="A122" s="58"/>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" ht="13.2">
       <c r="A123" s="58"/>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" ht="13.2">
       <c r="A124" s="58"/>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" ht="13.2">
       <c r="A125" s="58"/>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" ht="13.2">
       <c r="A126" s="58"/>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" ht="13.2">
       <c r="A127" s="58"/>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" ht="13.2">
       <c r="A128" s="58"/>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" ht="13.2">
       <c r="A129" s="58"/>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" ht="13.2">
       <c r="A130" s="58"/>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" ht="13.2">
       <c r="A131" s="58"/>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" ht="13.2">
       <c r="A132" s="58"/>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" ht="13.2">
       <c r="A133" s="58"/>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" ht="13.2">
       <c r="A134" s="58"/>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" ht="13.2">
       <c r="A135" s="58"/>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" ht="13.2">
       <c r="A136" s="58"/>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" ht="13.2">
       <c r="A137" s="58"/>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" ht="13.2">
       <c r="A138" s="58"/>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" ht="13.2">
       <c r="A139" s="58"/>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" ht="13.2">
       <c r="A140" s="58"/>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" ht="13.2">
       <c r="A141" s="58"/>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" ht="13.2">
       <c r="A142" s="58"/>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" ht="13.2">
       <c r="A143" s="58"/>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" ht="13.2">
       <c r="A144" s="58"/>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" ht="13.2">
       <c r="A145" s="58"/>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" ht="13.2">
       <c r="A146" s="58"/>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" ht="13.2">
       <c r="A147" s="58"/>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" ht="13.2">
       <c r="A148" s="58"/>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" ht="13.2">
       <c r="A149" s="58"/>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" ht="13.2">
       <c r="A150" s="58"/>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" ht="13.2">
       <c r="A151" s="58"/>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" ht="13.2">
       <c r="A152" s="58"/>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" ht="13.2">
       <c r="A153" s="58"/>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" ht="13.2">
       <c r="A154" s="58"/>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" ht="13.2">
       <c r="A155" s="58"/>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" ht="13.2">
       <c r="A156" s="58"/>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" ht="13.2">
       <c r="A157" s="58"/>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" ht="13.2">
       <c r="A158" s="58"/>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" ht="13.2">
       <c r="A159" s="58"/>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" ht="13.2">
       <c r="A160" s="58"/>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" ht="13.2">
       <c r="A161" s="58"/>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" ht="13.2">
       <c r="A162" s="58"/>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" ht="13.2">
       <c r="A163" s="58"/>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" ht="13.2">
       <c r="A164" s="58"/>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" ht="13.2">
       <c r="A165" s="58"/>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" ht="13.2">
       <c r="A166" s="58"/>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" ht="13.2">
       <c r="A167" s="58"/>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" ht="13.2">
       <c r="A168" s="58"/>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" ht="13.2">
       <c r="A169" s="58"/>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" ht="13.2">
       <c r="A170" s="58"/>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" ht="13.2">
       <c r="A171" s="58"/>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" ht="13.2">
       <c r="A172" s="58"/>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" ht="13.2">
       <c r="A173" s="58"/>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" ht="13.2">
       <c r="A174" s="58"/>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" ht="13.2">
       <c r="A175" s="58"/>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" ht="13.2">
       <c r="A176" s="58"/>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" ht="13.2">
       <c r="A177" s="58"/>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" ht="13.2">
       <c r="A178" s="58"/>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" ht="13.2">
       <c r="A179" s="58"/>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" ht="13.2">
       <c r="A180" s="58"/>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" ht="13.2">
       <c r="A181" s="58"/>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" ht="13.2">
       <c r="A182" s="58"/>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" ht="13.2">
       <c r="A183" s="58"/>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" ht="13.2">
       <c r="A184" s="58"/>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" ht="13.2">
       <c r="A185" s="58"/>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" ht="13.2">
       <c r="A186" s="58"/>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" ht="13.2">
       <c r="A187" s="58"/>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" ht="13.2">
       <c r="A188" s="58"/>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" ht="13.2">
       <c r="A189" s="58"/>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" ht="13.2">
       <c r="A190" s="58"/>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" ht="13.2">
       <c r="A191" s="58"/>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" ht="13.2">
       <c r="A192" s="58"/>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" ht="13.2">
       <c r="A193" s="58"/>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" ht="13.2">
       <c r="A194" s="58"/>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" ht="13.2">
       <c r="A195" s="58"/>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" ht="13.2">
       <c r="A196" s="58"/>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" ht="13.2">
       <c r="A197" s="58"/>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" ht="13.2">
       <c r="A198" s="58"/>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" ht="13.2">
       <c r="A199" s="58"/>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" ht="13.2">
       <c r="A200" s="58"/>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" ht="13.2">
       <c r="A201" s="58"/>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" ht="13.2">
       <c r="A202" s="58"/>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" ht="13.2">
       <c r="A203" s="58"/>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" ht="13.2">
       <c r="A204" s="58"/>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" ht="13.2">
       <c r="A205" s="58"/>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" ht="13.2">
       <c r="A206" s="58"/>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" ht="13.2">
       <c r="A207" s="58"/>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" ht="13.2">
       <c r="A208" s="58"/>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" ht="13.2">
       <c r="A209" s="58"/>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" ht="13.2">
       <c r="A210" s="58"/>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" ht="13.2">
       <c r="A211" s="58"/>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" ht="13.2">
       <c r="A212" s="58"/>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" ht="13.2">
       <c r="A213" s="58"/>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" ht="13.2">
       <c r="A214" s="58"/>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" ht="13.2">
       <c r="A215" s="58"/>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" ht="13.2">
       <c r="A216" s="58"/>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" ht="13.2">
       <c r="A217" s="58"/>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" ht="13.2">
       <c r="A218" s="58"/>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" ht="13.2">
       <c r="A219" s="58"/>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" ht="13.2">
       <c r="A220" s="58"/>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" ht="13.2">
       <c r="A221" s="58"/>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" ht="13.2">
       <c r="A222" s="58"/>
     </row>
-    <row r="223" spans="1:1">
+    <row r="223" spans="1:1" ht="13.2">
       <c r="A223" s="58"/>
     </row>
-    <row r="224" spans="1:1">
+    <row r="224" spans="1:1" ht="13.2">
       <c r="A224" s="58"/>
     </row>
-    <row r="225" spans="1:1">
+    <row r="225" spans="1:1" ht="13.2">
       <c r="A225" s="58"/>
     </row>
-    <row r="226" spans="1:1">
+    <row r="226" spans="1:1" ht="13.2">
       <c r="A226" s="58"/>
     </row>
-    <row r="227" spans="1:1">
+    <row r="227" spans="1:1" ht="13.2">
       <c r="A227" s="58"/>
     </row>
-    <row r="228" spans="1:1">
+    <row r="228" spans="1:1" ht="13.2">
       <c r="A228" s="58"/>
     </row>
-    <row r="229" spans="1:1">
+    <row r="229" spans="1:1" ht="13.2">
       <c r="A229" s="58"/>
     </row>
-    <row r="230" spans="1:1">
+    <row r="230" spans="1:1" ht="13.2">
       <c r="A230" s="58"/>
     </row>
-    <row r="231" spans="1:1">
+    <row r="231" spans="1:1" ht="13.2">
       <c r="A231" s="58"/>
     </row>
-    <row r="232" spans="1:1">
+    <row r="232" spans="1:1" ht="13.2">
       <c r="A232" s="58"/>
     </row>
-    <row r="233" spans="1:1">
+    <row r="233" spans="1:1" ht="13.2">
       <c r="A233" s="58"/>
     </row>
-    <row r="234" spans="1:1">
+    <row r="234" spans="1:1" ht="13.2">
       <c r="A234" s="58"/>
     </row>
-    <row r="235" spans="1:1">
+    <row r="235" spans="1:1" ht="13.2">
       <c r="A235" s="58"/>
     </row>
-    <row r="236" spans="1:1">
+    <row r="236" spans="1:1" ht="13.2">
       <c r="A236" s="58"/>
     </row>
-    <row r="237" spans="1:1">
+    <row r="237" spans="1:1" ht="13.2">
       <c r="A237" s="58"/>
     </row>
-    <row r="238" spans="1:1">
+    <row r="238" spans="1:1" ht="13.2">
       <c r="A238" s="58"/>
     </row>
-    <row r="239" spans="1:1">
+    <row r="239" spans="1:1" ht="13.2">
       <c r="A239" s="58"/>
     </row>
-    <row r="240" spans="1:1">
+    <row r="240" spans="1:1" ht="13.2">
       <c r="A240" s="58"/>
     </row>
-    <row r="241" spans="1:1">
+    <row r="241" spans="1:1" ht="13.2">
       <c r="A241" s="58"/>
     </row>
-    <row r="242" spans="1:1">
+    <row r="242" spans="1:1" ht="13.2">
       <c r="A242" s="58"/>
     </row>
-    <row r="243" spans="1:1">
+    <row r="243" spans="1:1" ht="13.2">
       <c r="A243" s="58"/>
     </row>
-    <row r="244" spans="1:1">
+    <row r="244" spans="1:1" ht="13.2">
       <c r="A244" s="58"/>
     </row>
-    <row r="245" spans="1:1">
+    <row r="245" spans="1:1" ht="13.2">
       <c r="A245" s="58"/>
     </row>
-    <row r="246" spans="1:1">
+    <row r="246" spans="1:1" ht="13.2">
       <c r="A246" s="58"/>
     </row>
-    <row r="247" spans="1:1">
+    <row r="247" spans="1:1" ht="13.2">
       <c r="A247" s="58"/>
     </row>
-    <row r="248" spans="1:1">
+    <row r="248" spans="1:1" ht="13.2">
       <c r="A248" s="58"/>
     </row>
-    <row r="249" spans="1:1">
+    <row r="249" spans="1:1" ht="13.2">
       <c r="A249" s="58"/>
     </row>
-    <row r="250" spans="1:1">
+    <row r="250" spans="1:1" ht="13.2">
       <c r="A250" s="58"/>
     </row>
-    <row r="251" spans="1:1">
+    <row r="251" spans="1:1" ht="13.2">
       <c r="A251" s="58"/>
     </row>
-    <row r="252" spans="1:1">
+    <row r="252" spans="1:1" ht="13.2">
       <c r="A252" s="58"/>
     </row>
-    <row r="253" spans="1:1">
+    <row r="253" spans="1:1" ht="13.2">
       <c r="A253" s="58"/>
     </row>
-    <row r="254" spans="1:1">
+    <row r="254" spans="1:1" ht="13.2">
       <c r="A254" s="58"/>
     </row>
-    <row r="255" spans="1:1">
+    <row r="255" spans="1:1" ht="13.2">
       <c r="A255" s="58"/>
     </row>
-    <row r="256" spans="1:1">
+    <row r="256" spans="1:1" ht="13.2">
       <c r="A256" s="58"/>
     </row>
-    <row r="257" spans="1:1">
+    <row r="257" spans="1:1" ht="13.2">
       <c r="A257" s="58"/>
     </row>
-    <row r="258" spans="1:1">
+    <row r="258" spans="1:1" ht="13.2">
       <c r="A258" s="58"/>
     </row>
-    <row r="259" spans="1:1">
+    <row r="259" spans="1:1" ht="13.2">
       <c r="A259" s="58"/>
     </row>
-    <row r="260" spans="1:1">
+    <row r="260" spans="1:1" ht="13.2">
       <c r="A260" s="58"/>
     </row>
-    <row r="261" spans="1:1">
+    <row r="261" spans="1:1" ht="13.2">
       <c r="A261" s="58"/>
     </row>
-    <row r="262" spans="1:1">
+    <row r="262" spans="1:1" ht="13.2">
       <c r="A262" s="58"/>
     </row>
-    <row r="263" spans="1:1">
+    <row r="263" spans="1:1" ht="13.2">
       <c r="A263" s="58"/>
     </row>
-    <row r="264" spans="1:1">
+    <row r="264" spans="1:1" ht="13.2">
       <c r="A264" s="58"/>
     </row>
-    <row r="265" spans="1:1">
+    <row r="265" spans="1:1" ht="13.2">
       <c r="A265" s="58"/>
     </row>
-    <row r="266" spans="1:1">
+    <row r="266" spans="1:1" ht="13.2">
       <c r="A266" s="58"/>
     </row>
-    <row r="267" spans="1:1">
+    <row r="267" spans="1:1" ht="13.2">
       <c r="A267" s="58"/>
     </row>
-    <row r="268" spans="1:1">
+    <row r="268" spans="1:1" ht="13.2">
       <c r="A268" s="58"/>
     </row>
-    <row r="269" spans="1:1">
+    <row r="269" spans="1:1" ht="13.2">
       <c r="A269" s="58"/>
     </row>
-    <row r="270" spans="1:1">
+    <row r="270" spans="1:1" ht="13.2">
       <c r="A270" s="58"/>
     </row>
-    <row r="271" spans="1:1">
+    <row r="271" spans="1:1" ht="13.2">
       <c r="A271" s="58"/>
     </row>
-    <row r="272" spans="1:1">
+    <row r="272" spans="1:1" ht="13.2">
       <c r="A272" s="58"/>
     </row>
-    <row r="273" spans="1:1">
+    <row r="273" spans="1:1" ht="13.2">
       <c r="A273" s="58"/>
     </row>
-    <row r="274" spans="1:1">
+    <row r="274" spans="1:1" ht="13.2">
       <c r="A274" s="58"/>
     </row>
-    <row r="275" spans="1:1">
+    <row r="275" spans="1:1" ht="13.2">
       <c r="A275" s="58"/>
     </row>
-    <row r="276" spans="1:1">
+    <row r="276" spans="1:1" ht="13.2">
       <c r="A276" s="58"/>
     </row>
-    <row r="277" spans="1:1">
+    <row r="277" spans="1:1" ht="13.2">
       <c r="A277" s="58"/>
     </row>
-    <row r="278" spans="1:1">
+    <row r="278" spans="1:1" ht="13.2">
       <c r="A278" s="58"/>
     </row>
-    <row r="279" spans="1:1">
+    <row r="279" spans="1:1" ht="13.2">
       <c r="A279" s="58"/>
     </row>
-    <row r="280" spans="1:1">
+    <row r="280" spans="1:1" ht="13.2">
       <c r="A280" s="58"/>
     </row>
-    <row r="281" spans="1:1">
+    <row r="281" spans="1:1" ht="13.2">
       <c r="A281" s="58"/>
     </row>
-    <row r="282" spans="1:1">
+    <row r="282" spans="1:1" ht="13.2">
       <c r="A282" s="58"/>
     </row>
-    <row r="283" spans="1:1">
+    <row r="283" spans="1:1" ht="13.2">
       <c r="A283" s="58"/>
     </row>
-    <row r="284" spans="1:1">
+    <row r="284" spans="1:1" ht="13.2">
       <c r="A284" s="58"/>
     </row>
-    <row r="285" spans="1:1">
+    <row r="285" spans="1:1" ht="13.2">
       <c r="A285" s="58"/>
     </row>
-    <row r="286" spans="1:1">
+    <row r="286" spans="1:1" ht="13.2">
       <c r="A286" s="58"/>
     </row>
-    <row r="287" spans="1:1">
+    <row r="287" spans="1:1" ht="13.2">
       <c r="A287" s="58"/>
     </row>
-    <row r="288" spans="1:1">
+    <row r="288" spans="1:1" ht="13.2">
       <c r="A288" s="58"/>
     </row>
-    <row r="289" spans="1:1">
+    <row r="289" spans="1:1" ht="13.2">
       <c r="A289" s="58"/>
     </row>
-    <row r="290" spans="1:1">
+    <row r="290" spans="1:1" ht="13.2">
       <c r="A290" s="58"/>
     </row>
-    <row r="291" spans="1:1">
+    <row r="291" spans="1:1" ht="13.2">
       <c r="A291" s="58"/>
     </row>
-    <row r="292" spans="1:1">
+    <row r="292" spans="1:1" ht="13.2">
       <c r="A292" s="58"/>
     </row>
-    <row r="293" spans="1:1">
+    <row r="293" spans="1:1" ht="13.2">
       <c r="A293" s="58"/>
     </row>
-    <row r="294" spans="1:1">
+    <row r="294" spans="1:1" ht="13.2">
       <c r="A294" s="58"/>
     </row>
-    <row r="295" spans="1:1">
+    <row r="295" spans="1:1" ht="13.2">
       <c r="A295" s="58"/>
     </row>
-    <row r="296" spans="1:1">
+    <row r="296" spans="1:1" ht="13.2">
       <c r="A296" s="58"/>
     </row>
-    <row r="297" spans="1:1">
+    <row r="297" spans="1:1" ht="13.2">
       <c r="A297" s="58"/>
     </row>
-    <row r="298" spans="1:1">
+    <row r="298" spans="1:1" ht="13.2">
       <c r="A298" s="58"/>
     </row>
-    <row r="299" spans="1:1">
+    <row r="299" spans="1:1" ht="13.2">
       <c r="A299" s="58"/>
     </row>
-    <row r="300" spans="1:1">
+    <row r="300" spans="1:1" ht="13.2">
       <c r="A300" s="58"/>
     </row>
-    <row r="301" spans="1:1">
+    <row r="301" spans="1:1" ht="13.2">
       <c r="A301" s="58"/>
     </row>
-    <row r="302" spans="1:1">
+    <row r="302" spans="1:1" ht="13.2">
       <c r="A302" s="58"/>
     </row>
-    <row r="303" spans="1:1">
+    <row r="303" spans="1:1" ht="13.2">
       <c r="A303" s="58"/>
     </row>
-    <row r="304" spans="1:1">
+    <row r="304" spans="1:1" ht="13.2">
       <c r="A304" s="58"/>
     </row>
-    <row r="305" spans="1:1">
+    <row r="305" spans="1:1" ht="13.2">
       <c r="A305" s="58"/>
     </row>
-    <row r="306" spans="1:1">
+    <row r="306" spans="1:1" ht="13.2">
       <c r="A306" s="58"/>
     </row>
-    <row r="307" spans="1:1">
+    <row r="307" spans="1:1" ht="13.2">
       <c r="A307" s="58"/>
     </row>
-    <row r="308" spans="1:1">
+    <row r="308" spans="1:1" ht="13.2">
       <c r="A308" s="58"/>
     </row>
-    <row r="309" spans="1:1">
+    <row r="309" spans="1:1" ht="13.2">
       <c r="A309" s="58"/>
     </row>
-    <row r="310" spans="1:1">
+    <row r="310" spans="1:1" ht="13.2">
       <c r="A310" s="58"/>
     </row>
-    <row r="311" spans="1:1">
+    <row r="311" spans="1:1" ht="13.2">
       <c r="A311" s="58"/>
     </row>
-    <row r="312" spans="1:1">
+    <row r="312" spans="1:1" ht="13.2">
       <c r="A312" s="58"/>
     </row>
-    <row r="313" spans="1:1">
+    <row r="313" spans="1:1" ht="13.2">
       <c r="A313" s="58"/>
     </row>
-    <row r="314" spans="1:1">
+    <row r="314" spans="1:1" ht="13.2">
       <c r="A314" s="58"/>
     </row>
-    <row r="315" spans="1:1">
+    <row r="315" spans="1:1" ht="13.2">
       <c r="A315" s="58"/>
     </row>
-    <row r="316" spans="1:1">
+    <row r="316" spans="1:1" ht="13.2">
       <c r="A316" s="58"/>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:1" ht="13.2">
       <c r="A317" s="58"/>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:1" ht="13.2">
       <c r="A318" s="58"/>
     </row>
-    <row r="319" spans="1:1">
+    <row r="319" spans="1:1" ht="13.2">
       <c r="A319" s="58"/>
     </row>
-    <row r="320" spans="1:1">
+    <row r="320" spans="1:1" ht="13.2">
       <c r="A320" s="58"/>
     </row>
-    <row r="321" spans="1:1">
+    <row r="321" spans="1:1" ht="13.2">
       <c r="A321" s="58"/>
     </row>
-    <row r="322" spans="1:1">
+    <row r="322" spans="1:1" ht="13.2">
       <c r="A322" s="58"/>
     </row>
-    <row r="323" spans="1:1">
+    <row r="323" spans="1:1" ht="13.2">
       <c r="A323" s="58"/>
     </row>
-    <row r="324" spans="1:1">
+    <row r="324" spans="1:1" ht="13.2">
       <c r="A324" s="58"/>
     </row>
-    <row r="325" spans="1:1">
+    <row r="325" spans="1:1" ht="13.2">
       <c r="A325" s="58"/>
     </row>
-    <row r="326" spans="1:1">
+    <row r="326" spans="1:1" ht="13.2">
       <c r="A326" s="58"/>
     </row>
-    <row r="327" spans="1:1">
+    <row r="327" spans="1:1" ht="13.2">
       <c r="A327" s="58"/>
     </row>
-    <row r="328" spans="1:1">
+    <row r="328" spans="1:1" ht="13.2">
       <c r="A328" s="58"/>
     </row>
-    <row r="329" spans="1:1">
+    <row r="329" spans="1:1" ht="13.2">
       <c r="A329" s="58"/>
     </row>
-    <row r="330" spans="1:1">
+    <row r="330" spans="1:1" ht="13.2">
       <c r="A330" s="58"/>
     </row>
-    <row r="331" spans="1:1">
+    <row r="331" spans="1:1" ht="13.2">
       <c r="A331" s="58"/>
     </row>
-    <row r="332" spans="1:1">
+    <row r="332" spans="1:1" ht="13.2">
       <c r="A332" s="58"/>
     </row>
-    <row r="333" spans="1:1">
+    <row r="333" spans="1:1" ht="13.2">
       <c r="A333" s="58"/>
     </row>
-    <row r="334" spans="1:1">
+    <row r="334" spans="1:1" ht="13.2">
       <c r="A334" s="58"/>
     </row>
-    <row r="335" spans="1:1">
+    <row r="335" spans="1:1" ht="13.2">
       <c r="A335" s="58"/>
     </row>
-    <row r="336" spans="1:1">
+    <row r="336" spans="1:1" ht="13.2">
       <c r="A336" s="58"/>
     </row>
-    <row r="337" spans="1:1">
+    <row r="337" spans="1:1" ht="13.2">
       <c r="A337" s="58"/>
     </row>
-    <row r="338" spans="1:1">
+    <row r="338" spans="1:1" ht="13.2">
       <c r="A338" s="58"/>
     </row>
-    <row r="339" spans="1:1">
+    <row r="339" spans="1:1" ht="13.2">
       <c r="A339" s="58"/>
     </row>
-    <row r="340" spans="1:1">
+    <row r="340" spans="1:1" ht="13.2">
       <c r="A340" s="58"/>
     </row>
-    <row r="341" spans="1:1">
+    <row r="341" spans="1:1" ht="13.2">
       <c r="A341" s="58"/>
     </row>
-    <row r="342" spans="1:1">
+    <row r="342" spans="1:1" ht="13.2">
       <c r="A342" s="58"/>
     </row>
-    <row r="343" spans="1:1">
+    <row r="343" spans="1:1" ht="13.2">
       <c r="A343" s="58"/>
     </row>
-    <row r="344" spans="1:1">
+    <row r="344" spans="1:1" ht="13.2">
       <c r="A344" s="58"/>
     </row>
-    <row r="345" spans="1:1">
+    <row r="345" spans="1:1" ht="13.2">
       <c r="A345" s="58"/>
     </row>
-    <row r="346" spans="1:1">
+    <row r="346" spans="1:1" ht="13.2">
       <c r="A346" s="58"/>
     </row>
-    <row r="347" spans="1:1">
+    <row r="347" spans="1:1" ht="13.2">
       <c r="A347" s="58"/>
     </row>
-    <row r="348" spans="1:1">
+    <row r="348" spans="1:1" ht="13.2">
       <c r="A348" s="58"/>
     </row>
-    <row r="349" spans="1:1">
+    <row r="349" spans="1:1" ht="13.2">
       <c r="A349" s="58"/>
     </row>
-    <row r="350" spans="1:1">
+    <row r="350" spans="1:1" ht="13.2">
       <c r="A350" s="58"/>
     </row>
-    <row r="351" spans="1:1">
+    <row r="351" spans="1:1" ht="13.2">
       <c r="A351" s="58"/>
     </row>
-    <row r="352" spans="1:1">
+    <row r="352" spans="1:1" ht="13.2">
       <c r="A352" s="58"/>
     </row>
-    <row r="353" spans="1:1">
+    <row r="353" spans="1:1" ht="13.2">
       <c r="A353" s="58"/>
     </row>
-    <row r="354" spans="1:1">
+    <row r="354" spans="1:1" ht="13.2">
       <c r="A354" s="58"/>
     </row>
-    <row r="355" spans="1:1">
+    <row r="355" spans="1:1" ht="13.2">
       <c r="A355" s="58"/>
     </row>
-    <row r="356" spans="1:1">
+    <row r="356" spans="1:1" ht="13.2">
       <c r="A356" s="58"/>
     </row>
-    <row r="357" spans="1:1">
+    <row r="357" spans="1:1" ht="13.2">
       <c r="A357" s="58"/>
     </row>
-    <row r="358" spans="1:1">
+    <row r="358" spans="1:1" ht="13.2">
       <c r="A358" s="58"/>
     </row>
-    <row r="359" spans="1:1">
+    <row r="359" spans="1:1" ht="13.2">
       <c r="A359" s="58"/>
     </row>
-    <row r="360" spans="1:1">
+    <row r="360" spans="1:1" ht="13.2">
       <c r="A360" s="58"/>
     </row>
-    <row r="361" spans="1:1">
+    <row r="361" spans="1:1" ht="13.2">
       <c r="A361" s="58"/>
     </row>
-    <row r="362" spans="1:1">
+    <row r="362" spans="1:1" ht="13.2">
       <c r="A362" s="58"/>
     </row>
-    <row r="363" spans="1:1">
+    <row r="363" spans="1:1" ht="13.2">
       <c r="A363" s="58"/>
     </row>
-    <row r="364" spans="1:1">
+    <row r="364" spans="1:1" ht="13.2">
       <c r="A364" s="58"/>
     </row>
-    <row r="365" spans="1:1">
+    <row r="365" spans="1:1" ht="13.2">
       <c r="A365" s="58"/>
     </row>
-    <row r="366" spans="1:1">
+    <row r="366" spans="1:1" ht="13.2">
       <c r="A366" s="58"/>
     </row>
-    <row r="367" spans="1:1">
+    <row r="367" spans="1:1" ht="13.2">
       <c r="A367" s="58"/>
     </row>
-    <row r="368" spans="1:1">
+    <row r="368" spans="1:1" ht="13.2">
       <c r="A368" s="58"/>
     </row>
-    <row r="369" spans="1:1">
+    <row r="369" spans="1:1" ht="13.2">
       <c r="A369" s="58"/>
     </row>
-    <row r="370" spans="1:1">
+    <row r="370" spans="1:1" ht="13.2">
       <c r="A370" s="58"/>
     </row>
-    <row r="371" spans="1:1">
+    <row r="371" spans="1:1" ht="13.2">
       <c r="A371" s="58"/>
     </row>
-    <row r="372" spans="1:1">
+    <row r="372" spans="1:1" ht="13.2">
       <c r="A372" s="58"/>
     </row>
-    <row r="373" spans="1:1">
+    <row r="373" spans="1:1" ht="13.2">
       <c r="A373" s="58"/>
     </row>
-    <row r="374" spans="1:1">
+    <row r="374" spans="1:1" ht="13.2">
       <c r="A374" s="58"/>
     </row>
-    <row r="375" spans="1:1">
+    <row r="375" spans="1:1" ht="13.2">
       <c r="A375" s="58"/>
     </row>
-    <row r="376" spans="1:1">
+    <row r="376" spans="1:1" ht="13.2">
       <c r="A376" s="58"/>
     </row>
-    <row r="377" spans="1:1">
+    <row r="377" spans="1:1" ht="13.2">
       <c r="A377" s="58"/>
     </row>
-    <row r="378" spans="1:1">
+    <row r="378" spans="1:1" ht="13.2">
       <c r="A378" s="58"/>
     </row>
-    <row r="379" spans="1:1">
+    <row r="379" spans="1:1" ht="13.2">
       <c r="A379" s="58"/>
     </row>
-    <row r="380" spans="1:1">
+    <row r="380" spans="1:1" ht="13.2">
       <c r="A380" s="58"/>
     </row>
-    <row r="381" spans="1:1">
+    <row r="381" spans="1:1" ht="13.2">
       <c r="A381" s="58"/>
     </row>
-    <row r="382" spans="1:1">
+    <row r="382" spans="1:1" ht="13.2">
       <c r="A382" s="58"/>
     </row>
-    <row r="383" spans="1:1">
+    <row r="383" spans="1:1" ht="13.2">
       <c r="A383" s="58"/>
     </row>
-    <row r="384" spans="1:1">
+    <row r="384" spans="1:1" ht="13.2">
       <c r="A384" s="58"/>
     </row>
-    <row r="385" spans="1:1">
+    <row r="385" spans="1:1" ht="13.2">
       <c r="A385" s="58"/>
     </row>
-    <row r="386" spans="1:1">
+    <row r="386" spans="1:1" ht="13.2">
       <c r="A386" s="58"/>
     </row>
-    <row r="387" spans="1:1">
+    <row r="387" spans="1:1" ht="13.2">
       <c r="A387" s="58"/>
     </row>
-    <row r="388" spans="1:1">
+    <row r="388" spans="1:1" ht="13.2">
       <c r="A388" s="58"/>
     </row>
-    <row r="389" spans="1:1">
+    <row r="389" spans="1:1" ht="13.2">
       <c r="A389" s="58"/>
     </row>
-    <row r="390" spans="1:1">
+    <row r="390" spans="1:1" ht="13.2">
       <c r="A390" s="58"/>
     </row>
-    <row r="391" spans="1:1">
+    <row r="391" spans="1:1" ht="13.2">
       <c r="A391" s="58"/>
     </row>
-    <row r="392" spans="1:1">
+    <row r="392" spans="1:1" ht="13.2">
       <c r="A392" s="58"/>
     </row>
-    <row r="393" spans="1:1">
+    <row r="393" spans="1:1" ht="13.2">
       <c r="A393" s="58"/>
     </row>
-    <row r="394" spans="1:1">
+    <row r="394" spans="1:1" ht="13.2">
       <c r="A394" s="58"/>
     </row>
-    <row r="395" spans="1:1">
+    <row r="395" spans="1:1" ht="13.2">
       <c r="A395" s="58"/>
     </row>
-    <row r="396" spans="1:1">
+    <row r="396" spans="1:1" ht="13.2">
       <c r="A396" s="58"/>
     </row>
-    <row r="397" spans="1:1">
+    <row r="397" spans="1:1" ht="13.2">
       <c r="A397" s="58"/>
     </row>
-    <row r="398" spans="1:1">
+    <row r="398" spans="1:1" ht="13.2">
       <c r="A398" s="58"/>
     </row>
-    <row r="399" spans="1:1">
+    <row r="399" spans="1:1" ht="13.2">
       <c r="A399" s="58"/>
     </row>
-    <row r="400" spans="1:1">
+    <row r="400" spans="1:1" ht="13.2">
       <c r="A400" s="58"/>
     </row>
-    <row r="401" spans="1:1">
+    <row r="401" spans="1:1" ht="13.2">
       <c r="A401" s="58"/>
     </row>
-    <row r="402" spans="1:1">
+    <row r="402" spans="1:1" ht="13.2">
       <c r="A402" s="58"/>
     </row>
-    <row r="403" spans="1:1">
+    <row r="403" spans="1:1" ht="13.2">
       <c r="A403" s="58"/>
     </row>
-    <row r="404" spans="1:1">
+    <row r="404" spans="1:1" ht="13.2">
       <c r="A404" s="58"/>
     </row>
-    <row r="405" spans="1:1">
+    <row r="405" spans="1:1" ht="13.2">
       <c r="A405" s="58"/>
     </row>
-    <row r="406" spans="1:1">
+    <row r="406" spans="1:1" ht="13.2">
       <c r="A406" s="58"/>
     </row>
-    <row r="407" spans="1:1">
+    <row r="407" spans="1:1" ht="13.2">
       <c r="A407" s="58"/>
     </row>
-    <row r="408" spans="1:1">
+    <row r="408" spans="1:1" ht="13.2">
       <c r="A408" s="58"/>
     </row>
-    <row r="409" spans="1:1">
+    <row r="409" spans="1:1" ht="13.2">
       <c r="A409" s="58"/>
     </row>
-    <row r="410" spans="1:1">
+    <row r="410" spans="1:1" ht="13.2">
       <c r="A410" s="58"/>
     </row>
-    <row r="411" spans="1:1">
+    <row r="411" spans="1:1" ht="13.2">
       <c r="A411" s="58"/>
     </row>
-    <row r="412" spans="1:1">
+    <row r="412" spans="1:1" ht="13.2">
       <c r="A412" s="58"/>
     </row>
-    <row r="413" spans="1:1">
+    <row r="413" spans="1:1" ht="13.2">
       <c r="A413" s="58"/>
     </row>
-    <row r="414" spans="1:1">
+    <row r="414" spans="1:1" ht="13.2">
       <c r="A414" s="58"/>
     </row>
-    <row r="415" spans="1:1">
+    <row r="415" spans="1:1" ht="13.2">
       <c r="A415" s="58"/>
     </row>
-    <row r="416" spans="1:1">
+    <row r="416" spans="1:1" ht="13.2">
       <c r="A416" s="58"/>
     </row>
-    <row r="417" spans="1:1">
+    <row r="417" spans="1:1" ht="13.2">
       <c r="A417" s="58"/>
     </row>
-    <row r="418" spans="1:1">
+    <row r="418" spans="1:1" ht="13.2">
       <c r="A418" s="58"/>
     </row>
-    <row r="419" spans="1:1">
+    <row r="419" spans="1:1" ht="13.2">
       <c r="A419" s="58"/>
     </row>
-    <row r="420" spans="1:1">
+    <row r="420" spans="1:1" ht="13.2">
       <c r="A420" s="58"/>
     </row>
-    <row r="421" spans="1:1">
+    <row r="421" spans="1:1" ht="13.2">
       <c r="A421" s="58"/>
     </row>
-    <row r="422" spans="1:1">
+    <row r="422" spans="1:1" ht="13.2">
       <c r="A422" s="58"/>
     </row>
-    <row r="423" spans="1:1">
+    <row r="423" spans="1:1" ht="13.2">
       <c r="A423" s="58"/>
     </row>
-    <row r="424" spans="1:1">
+    <row r="424" spans="1:1" ht="13.2">
       <c r="A424" s="58"/>
     </row>
-    <row r="425" spans="1:1">
+    <row r="425" spans="1:1" ht="13.2">
       <c r="A425" s="58"/>
     </row>
-    <row r="426" spans="1:1">
+    <row r="426" spans="1:1" ht="13.2">
       <c r="A426" s="58"/>
     </row>
-    <row r="427" spans="1:1">
+    <row r="427" spans="1:1" ht="13.2">
       <c r="A427" s="58"/>
     </row>
-    <row r="428" spans="1:1">
+    <row r="428" spans="1:1" ht="13.2">
       <c r="A428" s="58"/>
     </row>
-    <row r="429" spans="1:1">
+    <row r="429" spans="1:1" ht="13.2">
       <c r="A429" s="58"/>
     </row>
-    <row r="430" spans="1:1">
+    <row r="430" spans="1:1" ht="13.2">
       <c r="A430" s="58"/>
     </row>
-    <row r="431" spans="1:1">
+    <row r="431" spans="1:1" ht="13.2">
       <c r="A431" s="58"/>
     </row>
-    <row r="432" spans="1:1">
+    <row r="432" spans="1:1" ht="13.2">
       <c r="A432" s="58"/>
     </row>
-    <row r="433" spans="1:1">
+    <row r="433" spans="1:1" ht="13.2">
       <c r="A433" s="58"/>
     </row>
-    <row r="434" spans="1:1">
+    <row r="434" spans="1:1" ht="13.2">
       <c r="A434" s="58"/>
     </row>
-    <row r="435" spans="1:1">
+    <row r="435" spans="1:1" ht="13.2">
       <c r="A435" s="58"/>
     </row>
-    <row r="436" spans="1:1">
+    <row r="436" spans="1:1" ht="13.2">
       <c r="A436" s="58"/>
     </row>
-    <row r="437" spans="1:1">
+    <row r="437" spans="1:1" ht="13.2">
       <c r="A437" s="58"/>
     </row>
-    <row r="438" spans="1:1">
+    <row r="438" spans="1:1" ht="13.2">
       <c r="A438" s="58"/>
     </row>
-    <row r="439" spans="1:1">
+    <row r="439" spans="1:1" ht="13.2">
       <c r="A439" s="58"/>
     </row>
-    <row r="440" spans="1:1">
+    <row r="440" spans="1:1" ht="13.2">
       <c r="A440" s="58"/>
     </row>
-    <row r="441" spans="1:1">
+    <row r="441" spans="1:1" ht="13.2">
       <c r="A441" s="58"/>
     </row>
-    <row r="442" spans="1:1">
+    <row r="442" spans="1:1" ht="13.2">
       <c r="A442" s="58"/>
     </row>
-    <row r="443" spans="1:1">
+    <row r="443" spans="1:1" ht="13.2">
       <c r="A443" s="58"/>
     </row>
-    <row r="444" spans="1:1">
+    <row r="444" spans="1:1" ht="13.2">
       <c r="A444" s="58"/>
     </row>
-    <row r="445" spans="1:1">
+    <row r="445" spans="1:1" ht="13.2">
       <c r="A445" s="58"/>
     </row>
-    <row r="446" spans="1:1">
+    <row r="446" spans="1:1" ht="13.2">
       <c r="A446" s="58"/>
     </row>
-    <row r="447" spans="1:1">
+    <row r="447" spans="1:1" ht="13.2">
       <c r="A447" s="58"/>
     </row>
-    <row r="448" spans="1:1">
+    <row r="448" spans="1:1" ht="13.2">
       <c r="A448" s="58"/>
     </row>
-    <row r="449" spans="1:1">
+    <row r="449" spans="1:1" ht="13.2">
       <c r="A449" s="58"/>
     </row>
-    <row r="450" spans="1:1">
+    <row r="450" spans="1:1" ht="13.2">
       <c r="A450" s="58"/>
     </row>
-    <row r="451" spans="1:1">
+    <row r="451" spans="1:1" ht="13.2">
       <c r="A451" s="58"/>
     </row>
-    <row r="452" spans="1:1">
+    <row r="452" spans="1:1" ht="13.2">
       <c r="A452" s="58"/>
     </row>
-    <row r="453" spans="1:1">
+    <row r="453" spans="1:1" ht="13.2">
       <c r="A453" s="58"/>
     </row>
-    <row r="454" spans="1:1">
+    <row r="454" spans="1:1" ht="13.2">
       <c r="A454" s="58"/>
     </row>
-    <row r="455" spans="1:1">
+    <row r="455" spans="1:1" ht="13.2">
       <c r="A455" s="58"/>
     </row>
-    <row r="456" spans="1:1">
+    <row r="456" spans="1:1" ht="13.2">
       <c r="A456" s="58"/>
     </row>
-    <row r="457" spans="1:1">
+    <row r="457" spans="1:1" ht="13.2">
       <c r="A457" s="58"/>
     </row>
-    <row r="458" spans="1:1">
+    <row r="458" spans="1:1" ht="13.2">
       <c r="A458" s="58"/>
     </row>
-    <row r="459" spans="1:1">
+    <row r="459" spans="1:1" ht="13.2">
       <c r="A459" s="58"/>
     </row>
-    <row r="460" spans="1:1">
+    <row r="460" spans="1:1" ht="13.2">
       <c r="A460" s="58"/>
     </row>
-    <row r="461" spans="1:1">
+    <row r="461" spans="1:1" ht="13.2">
       <c r="A461" s="58"/>
     </row>
-    <row r="462" spans="1:1">
+    <row r="462" spans="1:1" ht="13.2">
       <c r="A462" s="58"/>
     </row>
-    <row r="463" spans="1:1">
+    <row r="463" spans="1:1" ht="13.2">
       <c r="A463" s="58"/>
     </row>
-    <row r="464" spans="1:1">
+    <row r="464" spans="1:1" ht="13.2">
       <c r="A464" s="58"/>
     </row>
-    <row r="465" spans="1:1">
+    <row r="465" spans="1:1" ht="13.2">
       <c r="A465" s="58"/>
     </row>
-    <row r="466" spans="1:1">
+    <row r="466" spans="1:1" ht="13.2">
       <c r="A466" s="58"/>
     </row>
-    <row r="467" spans="1:1">
+    <row r="467" spans="1:1" ht="13.2">
       <c r="A467" s="58"/>
     </row>
-    <row r="468" spans="1:1">
+    <row r="468" spans="1:1" ht="13.2">
       <c r="A468" s="58"/>
     </row>
-    <row r="469" spans="1:1">
+    <row r="469" spans="1:1" ht="13.2">
       <c r="A469" s="58"/>
     </row>
-    <row r="470" spans="1:1">
+    <row r="470" spans="1:1" ht="13.2">
       <c r="A470" s="58"/>
     </row>
-    <row r="471" spans="1:1">
+    <row r="471" spans="1:1" ht="13.2">
       <c r="A471" s="58"/>
     </row>
-    <row r="472" spans="1:1">
+    <row r="472" spans="1:1" ht="13.2">
       <c r="A472" s="58"/>
     </row>
-    <row r="473" spans="1:1">
+    <row r="473" spans="1:1" ht="13.2">
       <c r="A473" s="58"/>
     </row>
-    <row r="474" spans="1:1">
+    <row r="474" spans="1:1" ht="13.2">
       <c r="A474" s="58"/>
     </row>
-    <row r="475" spans="1:1">
+    <row r="475" spans="1:1" ht="13.2">
       <c r="A475" s="58"/>
     </row>
-    <row r="476" spans="1:1">
+    <row r="476" spans="1:1" ht="13.2">
       <c r="A476" s="58"/>
     </row>
-    <row r="477" spans="1:1">
+    <row r="477" spans="1:1" ht="13.2">
       <c r="A477" s="58"/>
     </row>
-    <row r="478" spans="1:1">
+    <row r="478" spans="1:1" ht="13.2">
       <c r="A478" s="58"/>
     </row>
-    <row r="479" spans="1:1">
+    <row r="479" spans="1:1" ht="13.2">
       <c r="A479" s="58"/>
     </row>
-    <row r="480" spans="1:1">
+    <row r="480" spans="1:1" ht="13.2">
       <c r="A480" s="58"/>
     </row>
-    <row r="481" spans="1:1">
+    <row r="481" spans="1:1" ht="13.2">
       <c r="A481" s="58"/>
     </row>
-    <row r="482" spans="1:1">
+    <row r="482" spans="1:1" ht="13.2">
       <c r="A482" s="58"/>
     </row>
-    <row r="483" spans="1:1">
+    <row r="483" spans="1:1" ht="13.2">
       <c r="A483" s="58"/>
     </row>
-    <row r="484" spans="1:1">
+    <row r="484" spans="1:1" ht="13.2">
       <c r="A484" s="58"/>
     </row>
-    <row r="485" spans="1:1">
+    <row r="485" spans="1:1" ht="13.2">
       <c r="A485" s="58"/>
     </row>
-    <row r="486" spans="1:1">
+    <row r="486" spans="1:1" ht="13.2">
       <c r="A486" s="58"/>
     </row>
-    <row r="487" spans="1:1">
+    <row r="487" spans="1:1" ht="13.2">
       <c r="A487" s="58"/>
     </row>
-    <row r="488" spans="1:1">
+    <row r="488" spans="1:1" ht="13.2">
       <c r="A488" s="58"/>
     </row>
-    <row r="489" spans="1:1">
+    <row r="489" spans="1:1" ht="13.2">
       <c r="A489" s="58"/>
     </row>
-    <row r="490" spans="1:1">
+    <row r="490" spans="1:1" ht="13.2">
       <c r="A490" s="58"/>
     </row>
-    <row r="491" spans="1:1">
+    <row r="491" spans="1:1" ht="13.2">
       <c r="A491" s="58"/>
     </row>
-    <row r="492" spans="1:1">
+    <row r="492" spans="1:1" ht="13.2">
       <c r="A492" s="58"/>
     </row>
-    <row r="493" spans="1:1">
+    <row r="493" spans="1:1" ht="13.2">
       <c r="A493" s="58"/>
     </row>
-    <row r="494" spans="1:1">
+    <row r="494" spans="1:1" ht="13.2">
       <c r="A494" s="58"/>
     </row>
-    <row r="495" spans="1:1">
+    <row r="495" spans="1:1" ht="13.2">
       <c r="A495" s="58"/>
     </row>
-    <row r="496" spans="1:1">
+    <row r="496" spans="1:1" ht="13.2">
       <c r="A496" s="58"/>
     </row>
-    <row r="497" spans="1:1">
+    <row r="497" spans="1:1" ht="13.2">
       <c r="A497" s="58"/>
     </row>
-    <row r="498" spans="1:1">
+    <row r="498" spans="1:1" ht="13.2">
       <c r="A498" s="58"/>
     </row>
-    <row r="499" spans="1:1">
+    <row r="499" spans="1:1" ht="13.2">
       <c r="A499" s="58"/>
     </row>
-    <row r="500" spans="1:1">
+    <row r="500" spans="1:1" ht="13.2">
       <c r="A500" s="58"/>
     </row>
-    <row r="501" spans="1:1">
+    <row r="501" spans="1:1" ht="13.2">
       <c r="A501" s="58"/>
     </row>
-    <row r="502" spans="1:1">
+    <row r="502" spans="1:1" ht="13.2">
       <c r="A502" s="58"/>
     </row>
-    <row r="503" spans="1:1">
+    <row r="503" spans="1:1" ht="13.2">
       <c r="A503" s="58"/>
     </row>
-    <row r="504" spans="1:1">
+    <row r="504" spans="1:1" ht="13.2">
       <c r="A504" s="58"/>
     </row>
-    <row r="505" spans="1:1">
+    <row r="505" spans="1:1" ht="13.2">
       <c r="A505" s="58"/>
     </row>
-    <row r="506" spans="1:1">
+    <row r="506" spans="1:1" ht="13.2">
       <c r="A506" s="58"/>
     </row>
-    <row r="507" spans="1:1">
+    <row r="507" spans="1:1" ht="13.2">
       <c r="A507" s="58"/>
     </row>
-    <row r="508" spans="1:1">
+    <row r="508" spans="1:1" ht="13.2">
       <c r="A508" s="58"/>
     </row>
-    <row r="509" spans="1:1">
+    <row r="509" spans="1:1" ht="13.2">
       <c r="A509" s="58"/>
     </row>
-    <row r="510" spans="1:1">
+    <row r="510" spans="1:1" ht="13.2">
       <c r="A510" s="58"/>
     </row>
-    <row r="511" spans="1:1">
+    <row r="511" spans="1:1" ht="13.2">
       <c r="A511" s="58"/>
     </row>
-    <row r="512" spans="1:1">
+    <row r="512" spans="1:1" ht="13.2">
       <c r="A512" s="58"/>
     </row>
-    <row r="513" spans="1:1">
+    <row r="513" spans="1:1" ht="13.2">
       <c r="A513" s="58"/>
     </row>
-    <row r="514" spans="1:1">
+    <row r="514" spans="1:1" ht="13.2">
       <c r="A514" s="58"/>
     </row>
-    <row r="515" spans="1:1">
+    <row r="515" spans="1:1" ht="13.2">
       <c r="A515" s="58"/>
     </row>
-    <row r="516" spans="1:1">
+    <row r="516" spans="1:1" ht="13.2">
       <c r="A516" s="58"/>
     </row>
-    <row r="517" spans="1:1">
+    <row r="517" spans="1:1" ht="13.2">
       <c r="A517" s="58"/>
     </row>
-    <row r="518" spans="1:1">
+    <row r="518" spans="1:1" ht="13.2">
       <c r="A518" s="58"/>
     </row>
-    <row r="519" spans="1:1">
+    <row r="519" spans="1:1" ht="13.2">
       <c r="A519" s="58"/>
     </row>
-    <row r="520" spans="1:1">
+    <row r="520" spans="1:1" ht="13.2">
       <c r="A520" s="58"/>
     </row>
-    <row r="521" spans="1:1">
+    <row r="521" spans="1:1" ht="13.2">
       <c r="A521" s="58"/>
     </row>
-    <row r="522" spans="1:1">
+    <row r="522" spans="1:1" ht="13.2">
       <c r="A522" s="58"/>
     </row>
-    <row r="523" spans="1:1">
+    <row r="523" spans="1:1" ht="13.2">
       <c r="A523" s="58"/>
     </row>
-    <row r="524" spans="1:1">
+    <row r="524" spans="1:1" ht="13.2">
       <c r="A524" s="58"/>
     </row>
-    <row r="525" spans="1:1">
+    <row r="525" spans="1:1" ht="13.2">
       <c r="A525" s="58"/>
     </row>
-    <row r="526" spans="1:1">
+    <row r="526" spans="1:1" ht="13.2">
       <c r="A526" s="58"/>
     </row>
-    <row r="527" spans="1:1">
+    <row r="527" spans="1:1" ht="13.2">
       <c r="A527" s="58"/>
     </row>
-    <row r="528" spans="1:1">
+    <row r="528" spans="1:1" ht="13.2">
       <c r="A528" s="58"/>
     </row>
-    <row r="529" spans="1:1">
+    <row r="529" spans="1:1" ht="13.2">
       <c r="A529" s="58"/>
     </row>
-    <row r="530" spans="1:1">
+    <row r="530" spans="1:1" ht="13.2">
       <c r="A530" s="58"/>
     </row>
-    <row r="531" spans="1:1">
+    <row r="531" spans="1:1" ht="13.2">
       <c r="A531" s="58"/>
     </row>
-    <row r="532" spans="1:1">
+    <row r="532" spans="1:1" ht="13.2">
       <c r="A532" s="58"/>
     </row>
-    <row r="533" spans="1:1">
+    <row r="533" spans="1:1" ht="13.2">
       <c r="A533" s="58"/>
     </row>
-    <row r="534" spans="1:1">
+    <row r="534" spans="1:1" ht="13.2">
       <c r="A534" s="58"/>
     </row>
-    <row r="535" spans="1:1">
+    <row r="535" spans="1:1" ht="13.2">
       <c r="A535" s="58"/>
     </row>
-    <row r="536" spans="1:1">
+    <row r="536" spans="1:1" ht="13.2">
       <c r="A536" s="58"/>
     </row>
-    <row r="537" spans="1:1">
+    <row r="537" spans="1:1" ht="13.2">
       <c r="A537" s="58"/>
     </row>
-    <row r="538" spans="1:1">
+    <row r="538" spans="1:1" ht="13.2">
       <c r="A538" s="58"/>
     </row>
-    <row r="539" spans="1:1">
+    <row r="539" spans="1:1" ht="13.2">
       <c r="A539" s="58"/>
     </row>
-    <row r="540" spans="1:1">
+    <row r="540" spans="1:1" ht="13.2">
       <c r="A540" s="58"/>
     </row>
-    <row r="541" spans="1:1">
+    <row r="541" spans="1:1" ht="13.2">
       <c r="A541" s="58"/>
     </row>
-    <row r="542" spans="1:1">
+    <row r="542" spans="1:1" ht="13.2">
       <c r="A542" s="58"/>
     </row>
-    <row r="543" spans="1:1">
+    <row r="543" spans="1:1" ht="13.2">
       <c r="A543" s="58"/>
     </row>
-    <row r="544" spans="1:1">
+    <row r="544" spans="1:1" ht="13.2">
       <c r="A544" s="58"/>
     </row>
-    <row r="545" spans="1:1">
+    <row r="545" spans="1:1" ht="13.2">
       <c r="A545" s="58"/>
     </row>
-    <row r="546" spans="1:1">
+    <row r="546" spans="1:1" ht="13.2">
       <c r="A546" s="58"/>
     </row>
-    <row r="547" spans="1:1">
+    <row r="547" spans="1:1" ht="13.2">
       <c r="A547" s="58"/>
     </row>
-    <row r="548" spans="1:1">
+    <row r="548" spans="1:1" ht="13.2">
       <c r="A548" s="58"/>
     </row>
-    <row r="549" spans="1:1">
+    <row r="549" spans="1:1" ht="13.2">
       <c r="A549" s="58"/>
     </row>
-    <row r="550" spans="1:1">
+    <row r="550" spans="1:1" ht="13.2">
       <c r="A550" s="58"/>
     </row>
-    <row r="551" spans="1:1">
+    <row r="551" spans="1:1" ht="13.2">
       <c r="A551" s="58"/>
     </row>
-    <row r="552" spans="1:1">
+    <row r="552" spans="1:1" ht="13.2">
       <c r="A552" s="58"/>
     </row>
-    <row r="553" spans="1:1">
+    <row r="553" spans="1:1" ht="13.2">
       <c r="A553" s="58"/>
     </row>
-    <row r="554" spans="1:1">
+    <row r="554" spans="1:1" ht="13.2">
       <c r="A554" s="58"/>
     </row>
-    <row r="555" spans="1:1">
+    <row r="555" spans="1:1" ht="13.2">
       <c r="A555" s="58"/>
     </row>
-    <row r="556" spans="1:1">
+    <row r="556" spans="1:1" ht="13.2">
       <c r="A556" s="58"/>
     </row>
-    <row r="557" spans="1:1">
+    <row r="557" spans="1:1" ht="13.2">
       <c r="A557" s="58"/>
     </row>
-    <row r="558" spans="1:1">
+    <row r="558" spans="1:1" ht="13.2">
       <c r="A558" s="58"/>
     </row>
-    <row r="559" spans="1:1">
+    <row r="559" spans="1:1" ht="13.2">
       <c r="A559" s="58"/>
     </row>
-    <row r="560" spans="1:1">
+    <row r="560" spans="1:1" ht="13.2">
       <c r="A560" s="58"/>
     </row>
-    <row r="561" spans="1:1">
+    <row r="561" spans="1:1" ht="13.2">
       <c r="A561" s="58"/>
     </row>
-    <row r="562" spans="1:1">
+    <row r="562" spans="1:1" ht="13.2">
       <c r="A562" s="58"/>
     </row>
-    <row r="563" spans="1:1">
+    <row r="563" spans="1:1" ht="13.2">
       <c r="A563" s="58"/>
     </row>
-    <row r="564" spans="1:1">
+    <row r="564" spans="1:1" ht="13.2">
       <c r="A564" s="58"/>
     </row>
-    <row r="565" spans="1:1">
+    <row r="565" spans="1:1" ht="13.2">
       <c r="A565" s="58"/>
     </row>
-    <row r="566" spans="1:1">
+    <row r="566" spans="1:1" ht="13.2">
       <c r="A566" s="58"/>
     </row>
-    <row r="567" spans="1:1">
+    <row r="567" spans="1:1" ht="13.2">
       <c r="A567" s="58"/>
     </row>
-    <row r="568" spans="1:1">
+    <row r="568" spans="1:1" ht="13.2">
       <c r="A568" s="58"/>
     </row>
-    <row r="569" spans="1:1">
+    <row r="569" spans="1:1" ht="13.2">
       <c r="A569" s="58"/>
     </row>
-    <row r="570" spans="1:1">
+    <row r="570" spans="1:1" ht="13.2">
       <c r="A570" s="58"/>
     </row>
-    <row r="571" spans="1:1">
+    <row r="571" spans="1:1" ht="13.2">
       <c r="A571" s="58"/>
     </row>
-    <row r="572" spans="1:1">
+    <row r="572" spans="1:1" ht="13.2">
       <c r="A572" s="58"/>
     </row>
-    <row r="573" spans="1:1">
+    <row r="573" spans="1:1" ht="13.2">
       <c r="A573" s="58"/>
     </row>
-    <row r="574" spans="1:1">
+    <row r="574" spans="1:1" ht="13.2">
       <c r="A574" s="58"/>
     </row>
-    <row r="575" spans="1:1">
+    <row r="575" spans="1:1" ht="13.2">
       <c r="A575" s="58"/>
     </row>
-    <row r="576" spans="1:1">
+    <row r="576" spans="1:1" ht="13.2">
       <c r="A576" s="58"/>
     </row>
-    <row r="577" spans="1:1">
+    <row r="577" spans="1:1" ht="13.2">
       <c r="A577" s="58"/>
     </row>
-    <row r="578" spans="1:1">
+    <row r="578" spans="1:1" ht="13.2">
       <c r="A578" s="58"/>
     </row>
-    <row r="579" spans="1:1">
+    <row r="579" spans="1:1" ht="13.2">
       <c r="A579" s="58"/>
     </row>
-    <row r="580" spans="1:1">
+    <row r="580" spans="1:1" ht="13.2">
       <c r="A580" s="58"/>
     </row>
-    <row r="581" spans="1:1">
+    <row r="581" spans="1:1" ht="13.2">
       <c r="A581" s="58"/>
     </row>
-    <row r="582" spans="1:1">
+    <row r="582" spans="1:1" ht="13.2">
       <c r="A582" s="58"/>
     </row>
-    <row r="583" spans="1:1">
+    <row r="583" spans="1:1" ht="13.2">
       <c r="A583" s="58"/>
     </row>
-    <row r="584" spans="1:1">
+    <row r="584" spans="1:1" ht="13.2">
       <c r="A584" s="58"/>
     </row>
-    <row r="585" spans="1:1">
+    <row r="585" spans="1:1" ht="13.2">
       <c r="A585" s="58"/>
     </row>
-    <row r="586" spans="1:1">
+    <row r="586" spans="1:1" ht="13.2">
       <c r="A586" s="58"/>
     </row>
-    <row r="587" spans="1:1">
+    <row r="587" spans="1:1" ht="13.2">
       <c r="A587" s="58"/>
     </row>
-    <row r="588" spans="1:1">
+    <row r="588" spans="1:1" ht="13.2">
       <c r="A588" s="58"/>
     </row>
-    <row r="589" spans="1:1">
+    <row r="589" spans="1:1" ht="13.2">
       <c r="A589" s="58"/>
     </row>
-    <row r="590" spans="1:1">
+    <row r="590" spans="1:1" ht="13.2">
       <c r="A590" s="58"/>
     </row>
-    <row r="591" spans="1:1">
+    <row r="591" spans="1:1" ht="13.2">
       <c r="A591" s="58"/>
     </row>
-    <row r="592" spans="1:1">
+    <row r="592" spans="1:1" ht="13.2">
       <c r="A592" s="58"/>
     </row>
-    <row r="593" spans="1:1">
+    <row r="593" spans="1:1" ht="13.2">
       <c r="A593" s="58"/>
     </row>
-    <row r="594" spans="1:1">
+    <row r="594" spans="1:1" ht="13.2">
       <c r="A594" s="58"/>
     </row>
-    <row r="595" spans="1:1">
+    <row r="595" spans="1:1" ht="13.2">
       <c r="A595" s="58"/>
     </row>
-    <row r="596" spans="1:1">
+    <row r="596" spans="1:1" ht="13.2">
       <c r="A596" s="58"/>
     </row>
-    <row r="597" spans="1:1">
+    <row r="597" spans="1:1" ht="13.2">
       <c r="A597" s="58"/>
     </row>
-    <row r="598" spans="1:1">
+    <row r="598" spans="1:1" ht="13.2">
       <c r="A598" s="58"/>
     </row>
-    <row r="599" spans="1:1">
+    <row r="599" spans="1:1" ht="13.2">
       <c r="A599" s="58"/>
     </row>
-    <row r="600" spans="1:1">
+    <row r="600" spans="1:1" ht="13.2">
       <c r="A600" s="58"/>
     </row>
-    <row r="601" spans="1:1">
+    <row r="601" spans="1:1" ht="13.2">
       <c r="A601" s="58"/>
     </row>
-    <row r="602" spans="1:1">
+    <row r="602" spans="1:1" ht="13.2">
       <c r="A602" s="58"/>
     </row>
-    <row r="603" spans="1:1">
+    <row r="603" spans="1:1" ht="13.2">
       <c r="A603" s="58"/>
     </row>
-    <row r="604" spans="1:1">
+    <row r="604" spans="1:1" ht="13.2">
       <c r="A604" s="58"/>
     </row>
-    <row r="605" spans="1:1">
+    <row r="605" spans="1:1" ht="13.2">
       <c r="A605" s="58"/>
     </row>
-    <row r="606" spans="1:1">
+    <row r="606" spans="1:1" ht="13.2">
       <c r="A606" s="58"/>
     </row>
-    <row r="607" spans="1:1">
+    <row r="607" spans="1:1" ht="13.2">
       <c r="A607" s="58"/>
     </row>
-    <row r="608" spans="1:1">
+    <row r="608" spans="1:1" ht="13.2">
       <c r="A608" s="58"/>
     </row>
-    <row r="609" spans="1:1">
+    <row r="609" spans="1:1" ht="13.2">
       <c r="A609" s="58"/>
     </row>
-    <row r="610" spans="1:1">
+    <row r="610" spans="1:1" ht="13.2">
       <c r="A610" s="58"/>
     </row>
-    <row r="611" spans="1:1">
+    <row r="611" spans="1:1" ht="13.2">
       <c r="A611" s="58"/>
     </row>
-    <row r="612" spans="1:1">
+    <row r="612" spans="1:1" ht="13.2">
       <c r="A612" s="58"/>
     </row>
-    <row r="613" spans="1:1">
+    <row r="613" spans="1:1" ht="13.2">
       <c r="A613" s="58"/>
     </row>
-    <row r="614" spans="1:1">
+    <row r="614" spans="1:1" ht="13.2">
       <c r="A614" s="58"/>
     </row>
-    <row r="615" spans="1:1">
+    <row r="615" spans="1:1" ht="13.2">
       <c r="A615" s="58"/>
     </row>
-    <row r="616" spans="1:1">
+    <row r="616" spans="1:1" ht="13.2">
       <c r="A616" s="58"/>
     </row>
-    <row r="617" spans="1:1">
+    <row r="617" spans="1:1" ht="13.2">
       <c r="A617" s="58"/>
     </row>
-    <row r="618" spans="1:1">
+    <row r="618" spans="1:1" ht="13.2">
       <c r="A618" s="58"/>
     </row>
-    <row r="619" spans="1:1">
+    <row r="619" spans="1:1" ht="13.2">
       <c r="A619" s="58"/>
     </row>
-    <row r="620" spans="1:1">
+    <row r="620" spans="1:1" ht="13.2">
       <c r="A620" s="58"/>
     </row>
-    <row r="621" spans="1:1">
+    <row r="621" spans="1:1" ht="13.2">
       <c r="A621" s="58"/>
     </row>
-    <row r="622" spans="1:1">
+    <row r="622" spans="1:1" ht="13.2">
       <c r="A622" s="58"/>
     </row>
-    <row r="623" spans="1:1">
+    <row r="623" spans="1:1" ht="13.2">
       <c r="A623" s="58"/>
     </row>
-    <row r="624" spans="1:1">
+    <row r="624" spans="1:1" ht="13.2">
       <c r="A624" s="58"/>
     </row>
-    <row r="625" spans="1:1">
+    <row r="625" spans="1:1" ht="13.2">
       <c r="A625" s="58"/>
     </row>
-    <row r="626" spans="1:1">
+    <row r="626" spans="1:1" ht="13.2">
       <c r="A626" s="58"/>
     </row>
-    <row r="627" spans="1:1">
+    <row r="627" spans="1:1" ht="13.2">
       <c r="A627" s="58"/>
     </row>
-    <row r="628" spans="1:1">
+    <row r="628" spans="1:1" ht="13.2">
       <c r="A628" s="58"/>
     </row>
-    <row r="629" spans="1:1">
+    <row r="629" spans="1:1" ht="13.2">
       <c r="A629" s="58"/>
     </row>
-    <row r="630" spans="1:1">
+    <row r="630" spans="1:1" ht="13.2">
       <c r="A630" s="58"/>
     </row>
-    <row r="631" spans="1:1">
+    <row r="631" spans="1:1" ht="13.2">
       <c r="A631" s="58"/>
     </row>
-    <row r="632" spans="1:1">
+    <row r="632" spans="1:1" ht="13.2">
       <c r="A632" s="58"/>
     </row>
-    <row r="633" spans="1:1">
+    <row r="633" spans="1:1" ht="13.2">
       <c r="A633" s="58"/>
     </row>
-    <row r="634" spans="1:1">
+    <row r="634" spans="1:1" ht="13.2">
       <c r="A634" s="58"/>
     </row>
-    <row r="635" spans="1:1">
+    <row r="635" spans="1:1" ht="13.2">
       <c r="A635" s="58"/>
     </row>
-    <row r="636" spans="1:1">
+    <row r="636" spans="1:1" ht="13.2">
       <c r="A636" s="58"/>
     </row>
-    <row r="637" spans="1:1">
+    <row r="637" spans="1:1" ht="13.2">
       <c r="A637" s="58"/>
     </row>
-    <row r="638" spans="1:1">
+    <row r="638" spans="1:1" ht="13.2">
       <c r="A638" s="58"/>
     </row>
-    <row r="639" spans="1:1">
+    <row r="639" spans="1:1" ht="13.2">
       <c r="A639" s="58"/>
     </row>
-    <row r="640" spans="1:1">
+    <row r="640" spans="1:1" ht="13.2">
       <c r="A640" s="58"/>
     </row>
-    <row r="641" spans="1:1">
+    <row r="641" spans="1:1" ht="13.2">
       <c r="A641" s="58"/>
     </row>
-    <row r="642" spans="1:1">
+    <row r="642" spans="1:1" ht="13.2">
       <c r="A642" s="58"/>
     </row>
-    <row r="643" spans="1:1">
+    <row r="643" spans="1:1" ht="13.2">
       <c r="A643" s="58"/>
     </row>
-    <row r="644" spans="1:1">
+    <row r="644" spans="1:1" ht="13.2">
       <c r="A644" s="58"/>
     </row>
-    <row r="645" spans="1:1">
+    <row r="645" spans="1:1" ht="13.2">
       <c r="A645" s="58"/>
     </row>
-    <row r="646" spans="1:1">
+    <row r="646" spans="1:1" ht="13.2">
       <c r="A646" s="58"/>
     </row>
-    <row r="647" spans="1:1">
+    <row r="647" spans="1:1" ht="13.2">
       <c r="A647" s="58"/>
     </row>
-    <row r="648" spans="1:1">
+    <row r="648" spans="1:1" ht="13.2">
       <c r="A648" s="58"/>
     </row>
-    <row r="649" spans="1:1">
+    <row r="649" spans="1:1" ht="13.2">
       <c r="A649" s="58"/>
     </row>
-    <row r="650" spans="1:1">
+    <row r="650" spans="1:1" ht="13.2">
       <c r="A650" s="58"/>
     </row>
-    <row r="651" spans="1:1">
+    <row r="651" spans="1:1" ht="13.2">
       <c r="A651" s="58"/>
     </row>
-    <row r="652" spans="1:1">
+    <row r="652" spans="1:1" ht="13.2">
       <c r="A652" s="58"/>
     </row>
-    <row r="653" spans="1:1">
+    <row r="653" spans="1:1" ht="13.2">
       <c r="A653" s="58"/>
     </row>
-    <row r="654" spans="1:1">
+    <row r="654" spans="1:1" ht="13.2">
       <c r="A654" s="58"/>
     </row>
-    <row r="655" spans="1:1">
+    <row r="655" spans="1:1" ht="13.2">
       <c r="A655" s="58"/>
     </row>
-    <row r="656" spans="1:1">
+    <row r="656" spans="1:1" ht="13.2">
       <c r="A656" s="58"/>
     </row>
-    <row r="657" spans="1:1">
+    <row r="657" spans="1:1" ht="13.2">
       <c r="A657" s="58"/>
     </row>
-    <row r="658" spans="1:1">
+    <row r="658" spans="1:1" ht="13.2">
       <c r="A658" s="58"/>
     </row>
-    <row r="659" spans="1:1">
+    <row r="659" spans="1:1" ht="13.2">
       <c r="A659" s="58"/>
     </row>
-    <row r="660" spans="1:1">
+    <row r="660" spans="1:1" ht="13.2">
       <c r="A660" s="58"/>
     </row>
-    <row r="661" spans="1:1">
+    <row r="661" spans="1:1" ht="13.2">
       <c r="A661" s="58"/>
     </row>
-    <row r="662" spans="1:1">
+    <row r="662" spans="1:1" ht="13.2">
       <c r="A662" s="58"/>
     </row>
-    <row r="663" spans="1:1">
+    <row r="663" spans="1:1" ht="13.2">
       <c r="A663" s="58"/>
     </row>
-    <row r="664" spans="1:1">
+    <row r="664" spans="1:1" ht="13.2">
       <c r="A664" s="58"/>
     </row>
-    <row r="665" spans="1:1">
+    <row r="665" spans="1:1" ht="13.2">
       <c r="A665" s="58"/>
     </row>
-    <row r="666" spans="1:1">
+    <row r="666" spans="1:1" ht="13.2">
       <c r="A666" s="58"/>
     </row>
-    <row r="667" spans="1:1">
+    <row r="667" spans="1:1" ht="13.2">
       <c r="A667" s="58"/>
     </row>
-    <row r="668" spans="1:1">
+    <row r="668" spans="1:1" ht="13.2">
       <c r="A668" s="58"/>
     </row>
-    <row r="669" spans="1:1">
+    <row r="669" spans="1:1" ht="13.2">
       <c r="A669" s="58"/>
     </row>
-    <row r="670" spans="1:1">
+    <row r="670" spans="1:1" ht="13.2">
       <c r="A670" s="58"/>
     </row>
-    <row r="671" spans="1:1">
+    <row r="671" spans="1:1" ht="13.2">
       <c r="A671" s="58"/>
     </row>
-    <row r="672" spans="1:1">
+    <row r="672" spans="1:1" ht="13.2">
       <c r="A672" s="58"/>
     </row>
-    <row r="673" spans="1:1">
+    <row r="673" spans="1:1" ht="13.2">
       <c r="A673" s="58"/>
     </row>
-    <row r="674" spans="1:1">
+    <row r="674" spans="1:1" ht="13.2">
       <c r="A674" s="58"/>
     </row>
-    <row r="675" spans="1:1">
+    <row r="675" spans="1:1" ht="13.2">
       <c r="A675" s="58"/>
     </row>
-    <row r="676" spans="1:1">
+    <row r="676" spans="1:1" ht="13.2">
       <c r="A676" s="58"/>
     </row>
-    <row r="677" spans="1:1">
+    <row r="677" spans="1:1" ht="13.2">
       <c r="A677" s="58"/>
     </row>
-    <row r="678" spans="1:1">
+    <row r="678" spans="1:1" ht="13.2">
       <c r="A678" s="58"/>
     </row>
-    <row r="679" spans="1:1">
+    <row r="679" spans="1:1" ht="13.2">
       <c r="A679" s="58"/>
     </row>
-    <row r="680" spans="1:1">
+    <row r="680" spans="1:1" ht="13.2">
       <c r="A680" s="58"/>
     </row>
-    <row r="681" spans="1:1">
+    <row r="681" spans="1:1" ht="13.2">
       <c r="A681" s="58"/>
     </row>
-    <row r="682" spans="1:1">
+    <row r="682" spans="1:1" ht="13.2">
       <c r="A682" s="58"/>
     </row>
-    <row r="683" spans="1:1">
+    <row r="683" spans="1:1" ht="13.2">
       <c r="A683" s="58"/>
     </row>
-    <row r="684" spans="1:1">
+    <row r="684" spans="1:1" ht="13.2">
       <c r="A684" s="58"/>
     </row>
-    <row r="685" spans="1:1">
+    <row r="685" spans="1:1" ht="13.2">
       <c r="A685" s="58"/>
     </row>
-    <row r="686" spans="1:1">
+    <row r="686" spans="1:1" ht="13.2">
       <c r="A686" s="58"/>
     </row>
-    <row r="687" spans="1:1">
+    <row r="687" spans="1:1" ht="13.2">
       <c r="A687" s="58"/>
     </row>
-    <row r="688" spans="1:1">
+    <row r="688" spans="1:1" ht="13.2">
       <c r="A688" s="58"/>
     </row>
-    <row r="689" spans="1:1">
+    <row r="689" spans="1:1" ht="13.2">
       <c r="A689" s="58"/>
     </row>
-    <row r="690" spans="1:1">
+    <row r="690" spans="1:1" ht="13.2">
       <c r="A690" s="58"/>
     </row>
-    <row r="691" spans="1:1">
+    <row r="691" spans="1:1" ht="13.2">
       <c r="A691" s="58"/>
     </row>
-    <row r="692" spans="1:1">
+    <row r="692" spans="1:1" ht="13.2">
       <c r="A692" s="58"/>
     </row>
-    <row r="693" spans="1:1">
+    <row r="693" spans="1:1" ht="13.2">
       <c r="A693" s="58"/>
     </row>
-    <row r="694" spans="1:1">
+    <row r="694" spans="1:1" ht="13.2">
       <c r="A694" s="58"/>
     </row>
-    <row r="695" spans="1:1">
+    <row r="695" spans="1:1" ht="13.2">
       <c r="A695" s="58"/>
     </row>
-    <row r="696" spans="1:1">
+    <row r="696" spans="1:1" ht="13.2">
       <c r="A696" s="58"/>
     </row>
-    <row r="697" spans="1:1">
+    <row r="697" spans="1:1" ht="13.2">
       <c r="A697" s="58"/>
     </row>
-    <row r="698" spans="1:1">
+    <row r="698" spans="1:1" ht="13.2">
       <c r="A698" s="58"/>
     </row>
-    <row r="699" spans="1:1">
+    <row r="699" spans="1:1" ht="13.2">
       <c r="A699" s="58"/>
     </row>
-    <row r="700" spans="1:1">
+    <row r="700" spans="1:1" ht="13.2">
       <c r="A700" s="58"/>
     </row>
-    <row r="701" spans="1:1">
+    <row r="701" spans="1:1" ht="13.2">
       <c r="A701" s="58"/>
     </row>
-    <row r="702" spans="1:1">
+    <row r="702" spans="1:1" ht="13.2">
       <c r="A702" s="58"/>
     </row>
-    <row r="703" spans="1:1">
+    <row r="703" spans="1:1" ht="13.2">
       <c r="A703" s="58"/>
     </row>
-    <row r="704" spans="1:1">
+    <row r="704" spans="1:1" ht="13.2">
       <c r="A704" s="58"/>
     </row>
-    <row r="705" spans="1:1">
+    <row r="705" spans="1:1" ht="13.2">
       <c r="A705" s="58"/>
     </row>
-    <row r="706" spans="1:1">
+    <row r="706" spans="1:1" ht="13.2">
       <c r="A706" s="58"/>
     </row>
-    <row r="707" spans="1:1">
+    <row r="707" spans="1:1" ht="13.2">
       <c r="A707" s="58"/>
     </row>
-    <row r="708" spans="1:1">
+    <row r="708" spans="1:1" ht="13.2">
       <c r="A708" s="58"/>
     </row>
-    <row r="709" spans="1:1">
+    <row r="709" spans="1:1" ht="13.2">
       <c r="A709" s="58"/>
     </row>
-    <row r="710" spans="1:1">
+    <row r="710" spans="1:1" ht="13.2">
       <c r="A710" s="58"/>
     </row>
-    <row r="711" spans="1:1">
+    <row r="711" spans="1:1" ht="13.2">
       <c r="A711" s="58"/>
     </row>
-    <row r="712" spans="1:1">
+    <row r="712" spans="1:1" ht="13.2">
       <c r="A712" s="58"/>
     </row>
-    <row r="713" spans="1:1">
+    <row r="713" spans="1:1" ht="13.2">
       <c r="A713" s="58"/>
     </row>
-    <row r="714" spans="1:1">
+    <row r="714" spans="1:1" ht="13.2">
       <c r="A714" s="58"/>
     </row>
-    <row r="715" spans="1:1">
+    <row r="715" spans="1:1" ht="13.2">
       <c r="A715" s="58"/>
     </row>
-    <row r="716" spans="1:1">
+    <row r="716" spans="1:1" ht="13.2">
       <c r="A716" s="58"/>
     </row>
-    <row r="717" spans="1:1">
+    <row r="717" spans="1:1" ht="13.2">
       <c r="A717" s="58"/>
     </row>
-    <row r="718" spans="1:1">
+    <row r="718" spans="1:1" ht="13.2">
       <c r="A718" s="58"/>
     </row>
-    <row r="719" spans="1:1">
+    <row r="719" spans="1:1" ht="13.2">
       <c r="A719" s="58"/>
     </row>
-    <row r="720" spans="1:1">
+    <row r="720" spans="1:1" ht="13.2">
       <c r="A720" s="58"/>
     </row>
-    <row r="721" spans="1:1">
+    <row r="721" spans="1:1" ht="13.2">
       <c r="A721" s="58"/>
     </row>
-    <row r="722" spans="1:1">
+    <row r="722" spans="1:1" ht="13.2">
       <c r="A722" s="58"/>
     </row>
-    <row r="723" spans="1:1">
+    <row r="723" spans="1:1" ht="13.2">
       <c r="A723" s="58"/>
     </row>
-    <row r="724" spans="1:1">
+    <row r="724" spans="1:1" ht="13.2">
       <c r="A724" s="58"/>
     </row>
-    <row r="725" spans="1:1">
+    <row r="725" spans="1:1" ht="13.2">
       <c r="A725" s="58"/>
     </row>
-    <row r="726" spans="1:1">
+    <row r="726" spans="1:1" ht="13.2">
       <c r="A726" s="58"/>
     </row>
-    <row r="727" spans="1:1">
+    <row r="727" spans="1:1" ht="13.2">
       <c r="A727" s="58"/>
     </row>
-    <row r="728" spans="1:1">
+    <row r="728" spans="1:1" ht="13.2">
       <c r="A728" s="58"/>
     </row>
-    <row r="729" spans="1:1">
+    <row r="729" spans="1:1" ht="13.2">
       <c r="A729" s="58"/>
     </row>
-    <row r="730" spans="1:1">
+    <row r="730" spans="1:1" ht="13.2">
       <c r="A730" s="58"/>
     </row>
-    <row r="731" spans="1:1">
+    <row r="731" spans="1:1" ht="13.2">
       <c r="A731" s="58"/>
     </row>
-    <row r="732" spans="1:1">
+    <row r="732" spans="1:1" ht="13.2">
       <c r="A732" s="58"/>
     </row>
-    <row r="733" spans="1:1">
+    <row r="733" spans="1:1" ht="13.2">
       <c r="A733" s="58"/>
     </row>
-    <row r="734" spans="1:1">
+    <row r="734" spans="1:1" ht="13.2">
       <c r="A734" s="58"/>
     </row>
-    <row r="735" spans="1:1">
+    <row r="735" spans="1:1" ht="13.2">
       <c r="A735" s="58"/>
     </row>
-    <row r="736" spans="1:1">
+    <row r="736" spans="1:1" ht="13.2">
       <c r="A736" s="58"/>
     </row>
-    <row r="737" spans="1:1">
+    <row r="737" spans="1:1" ht="13.2">
       <c r="A737" s="58"/>
     </row>
-    <row r="738" spans="1:1">
+    <row r="738" spans="1:1" ht="13.2">
       <c r="A738" s="58"/>
     </row>
-    <row r="739" spans="1:1">
+    <row r="739" spans="1:1" ht="13.2">
       <c r="A739" s="58"/>
     </row>
-    <row r="740" spans="1:1">
+    <row r="740" spans="1:1" ht="13.2">
       <c r="A740" s="58"/>
     </row>
-    <row r="741" spans="1:1">
+    <row r="741" spans="1:1" ht="13.2">
       <c r="A741" s="58"/>
     </row>
-    <row r="742" spans="1:1">
+    <row r="742" spans="1:1" ht="13.2">
       <c r="A742" s="58"/>
     </row>
-    <row r="743" spans="1:1">
+    <row r="743" spans="1:1" ht="13.2">
       <c r="A743" s="58"/>
     </row>
-    <row r="744" spans="1:1">
+    <row r="744" spans="1:1" ht="13.2">
       <c r="A744" s="58"/>
     </row>
-    <row r="745" spans="1:1">
+    <row r="745" spans="1:1" ht="13.2">
       <c r="A745" s="58"/>
     </row>
-    <row r="746" spans="1:1">
+    <row r="746" spans="1:1" ht="13.2">
       <c r="A746" s="58"/>
     </row>
-    <row r="747" spans="1:1">
+    <row r="747" spans="1:1" ht="13.2">
       <c r="A747" s="58"/>
     </row>
-    <row r="748" spans="1:1">
+    <row r="748" spans="1:1" ht="13.2">
       <c r="A748" s="58"/>
     </row>
-    <row r="749" spans="1:1">
+    <row r="749" spans="1:1" ht="13.2">
       <c r="A749" s="58"/>
     </row>
-    <row r="750" spans="1:1">
+    <row r="750" spans="1:1" ht="13.2">
       <c r="A750" s="58"/>
     </row>
-    <row r="751" spans="1:1">
+    <row r="751" spans="1:1" ht="13.2">
       <c r="A751" s="58"/>
     </row>
-    <row r="752" spans="1:1">
+    <row r="752" spans="1:1" ht="13.2">
       <c r="A752" s="58"/>
     </row>
-    <row r="753" spans="1:1">
+    <row r="753" spans="1:1" ht="13.2">
       <c r="A753" s="58"/>
     </row>
-    <row r="754" spans="1:1">
+    <row r="754" spans="1:1" ht="13.2">
       <c r="A754" s="58"/>
     </row>
-    <row r="755" spans="1:1">
+    <row r="755" spans="1:1" ht="13.2">
       <c r="A755" s="58"/>
     </row>
-    <row r="756" spans="1:1">
+    <row r="756" spans="1:1" ht="13.2">
       <c r="A756" s="58"/>
     </row>
-    <row r="757" spans="1:1">
+    <row r="757" spans="1:1" ht="13.2">
       <c r="A757" s="58"/>
     </row>
-    <row r="758" spans="1:1">
+    <row r="758" spans="1:1" ht="13.2">
       <c r="A758" s="58"/>
     </row>
-    <row r="759" spans="1:1">
+    <row r="759" spans="1:1" ht="13.2">
       <c r="A759" s="58"/>
     </row>
-    <row r="760" spans="1:1">
+    <row r="760" spans="1:1" ht="13.2">
       <c r="A760" s="58"/>
     </row>
-    <row r="761" spans="1:1">
+    <row r="761" spans="1:1" ht="13.2">
       <c r="A761" s="58"/>
     </row>
-    <row r="762" spans="1:1">
+    <row r="762" spans="1:1" ht="13.2">
       <c r="A762" s="58"/>
     </row>
-    <row r="763" spans="1:1">
+    <row r="763" spans="1:1" ht="13.2">
       <c r="A763" s="58"/>
     </row>
-    <row r="764" spans="1:1">
+    <row r="764" spans="1:1" ht="13.2">
       <c r="A764" s="58"/>
     </row>
-    <row r="765" spans="1:1">
+    <row r="765" spans="1:1" ht="13.2">
       <c r="A765" s="58"/>
     </row>
-    <row r="766" spans="1:1">
+    <row r="766" spans="1:1" ht="13.2">
       <c r="A766" s="58"/>
     </row>
-    <row r="767" spans="1:1">
+    <row r="767" spans="1:1" ht="13.2">
       <c r="A767" s="58"/>
     </row>
-    <row r="768" spans="1:1">
+    <row r="768" spans="1:1" ht="13.2">
       <c r="A768" s="58"/>
     </row>
-    <row r="769" spans="1:1">
+    <row r="769" spans="1:1" ht="13.2">
       <c r="A769" s="58"/>
     </row>
-    <row r="770" spans="1:1">
+    <row r="770" spans="1:1" ht="13.2">
       <c r="A770" s="58"/>
     </row>
-    <row r="771" spans="1:1">
+    <row r="771" spans="1:1" ht="13.2">
       <c r="A771" s="58"/>
     </row>
-    <row r="772" spans="1:1">
+    <row r="772" spans="1:1" ht="13.2">
       <c r="A772" s="58"/>
     </row>
-    <row r="773" spans="1:1">
+    <row r="773" spans="1:1" ht="13.2">
       <c r="A773" s="58"/>
     </row>
-    <row r="774" spans="1:1">
+    <row r="774" spans="1:1" ht="13.2">
       <c r="A774" s="58"/>
     </row>
-    <row r="775" spans="1:1">
+    <row r="775" spans="1:1" ht="13.2">
       <c r="A775" s="58"/>
     </row>
-    <row r="776" spans="1:1">
+    <row r="776" spans="1:1" ht="13.2">
       <c r="A776" s="58"/>
     </row>
-    <row r="777" spans="1:1">
+    <row r="777" spans="1:1" ht="13.2">
       <c r="A777" s="58"/>
     </row>
-    <row r="778" spans="1:1">
+    <row r="778" spans="1:1" ht="13.2">
       <c r="A778" s="58"/>
     </row>
-    <row r="779" spans="1:1">
+    <row r="779" spans="1:1" ht="13.2">
       <c r="A779" s="58"/>
     </row>
-    <row r="780" spans="1:1">
+    <row r="780" spans="1:1" ht="13.2">
       <c r="A780" s="58"/>
     </row>
-    <row r="781" spans="1:1">
+    <row r="781" spans="1:1" ht="13.2">
       <c r="A781" s="58"/>
     </row>
-    <row r="782" spans="1:1">
+    <row r="782" spans="1:1" ht="13.2">
       <c r="A782" s="58"/>
     </row>
-    <row r="783" spans="1:1">
+    <row r="783" spans="1:1" ht="13.2">
       <c r="A783" s="58"/>
     </row>
-    <row r="784" spans="1:1">
+    <row r="784" spans="1:1" ht="13.2">
       <c r="A784" s="58"/>
     </row>
-    <row r="785" spans="1:1">
+    <row r="785" spans="1:1" ht="13.2">
       <c r="A785" s="58"/>
     </row>
-    <row r="786" spans="1:1">
+    <row r="786" spans="1:1" ht="13.2">
       <c r="A786" s="58"/>
     </row>
-    <row r="787" spans="1:1">
+    <row r="787" spans="1:1" ht="13.2">
       <c r="A787" s="58"/>
     </row>
-    <row r="788" spans="1:1">
+    <row r="788" spans="1:1" ht="13.2">
       <c r="A788" s="58"/>
     </row>
-    <row r="789" spans="1:1">
+    <row r="789" spans="1:1" ht="13.2">
       <c r="A789" s="58"/>
     </row>
-    <row r="790" spans="1:1">
+    <row r="790" spans="1:1" ht="13.2">
       <c r="A790" s="58"/>
     </row>
-    <row r="791" spans="1:1">
+    <row r="791" spans="1:1" ht="13.2">
       <c r="A791" s="58"/>
     </row>
-    <row r="792" spans="1:1">
+    <row r="792" spans="1:1" ht="13.2">
       <c r="A792" s="58"/>
     </row>
-    <row r="793" spans="1:1">
+    <row r="793" spans="1:1" ht="13.2">
       <c r="A793" s="58"/>
     </row>
-    <row r="794" spans="1:1">
+    <row r="794" spans="1:1" ht="13.2">
       <c r="A794" s="58"/>
     </row>
-    <row r="795" spans="1:1">
+    <row r="795" spans="1:1" ht="13.2">
       <c r="A795" s="58"/>
     </row>
-    <row r="796" spans="1:1">
+    <row r="796" spans="1:1" ht="13.2">
       <c r="A796" s="58"/>
     </row>
-    <row r="797" spans="1:1">
+    <row r="797" spans="1:1" ht="13.2">
       <c r="A797" s="58"/>
     </row>
-    <row r="798" spans="1:1">
+    <row r="798" spans="1:1" ht="13.2">
       <c r="A798" s="58"/>
     </row>
-    <row r="799" spans="1:1">
+    <row r="799" spans="1:1" ht="13.2">
       <c r="A799" s="58"/>
     </row>
-    <row r="800" spans="1:1">
+    <row r="800" spans="1:1" ht="13.2">
       <c r="A800" s="58"/>
     </row>
-    <row r="801" spans="1:1">
+    <row r="801" spans="1:1" ht="13.2">
       <c r="A801" s="58"/>
     </row>
-    <row r="802" spans="1:1">
+    <row r="802" spans="1:1" ht="13.2">
       <c r="A802" s="58"/>
     </row>
-    <row r="803" spans="1:1">
+    <row r="803" spans="1:1" ht="13.2">
       <c r="A803" s="58"/>
     </row>
-    <row r="804" spans="1:1">
+    <row r="804" spans="1:1" ht="13.2">
       <c r="A804" s="58"/>
     </row>
-    <row r="805" spans="1:1">
+    <row r="805" spans="1:1" ht="13.2">
       <c r="A805" s="58"/>
     </row>
-    <row r="806" spans="1:1">
+    <row r="806" spans="1:1" ht="13.2">
       <c r="A806" s="58"/>
     </row>
-    <row r="807" spans="1:1">
+    <row r="807" spans="1:1" ht="13.2">
       <c r="A807" s="58"/>
     </row>
-    <row r="808" spans="1:1">
+    <row r="808" spans="1:1" ht="13.2">
       <c r="A808" s="58"/>
     </row>
-    <row r="809" spans="1:1">
+    <row r="809" spans="1:1" ht="13.2">
       <c r="A809" s="58"/>
     </row>
-    <row r="810" spans="1:1">
+    <row r="810" spans="1:1" ht="13.2">
       <c r="A810" s="58"/>
     </row>
-    <row r="811" spans="1:1">
+    <row r="811" spans="1:1" ht="13.2">
       <c r="A811" s="58"/>
     </row>
-    <row r="812" spans="1:1">
+    <row r="812" spans="1:1" ht="13.2">
       <c r="A812" s="58"/>
     </row>
-    <row r="813" spans="1:1">
+    <row r="813" spans="1:1" ht="13.2">
       <c r="A813" s="58"/>
     </row>
-    <row r="814" spans="1:1">
+    <row r="814" spans="1:1" ht="13.2">
       <c r="A814" s="58"/>
     </row>
-    <row r="815" spans="1:1">
+    <row r="815" spans="1:1" ht="13.2">
       <c r="A815" s="58"/>
     </row>
-    <row r="816" spans="1:1">
+    <row r="816" spans="1:1" ht="13.2">
       <c r="A816" s="58"/>
     </row>
-    <row r="817" spans="1:1">
+    <row r="817" spans="1:1" ht="13.2">
       <c r="A817" s="58"/>
     </row>
-    <row r="818" spans="1:1">
+    <row r="818" spans="1:1" ht="13.2">
       <c r="A818" s="58"/>
     </row>
-    <row r="819" spans="1:1">
+    <row r="819" spans="1:1" ht="13.2">
       <c r="A819" s="58"/>
     </row>
-    <row r="820" spans="1:1">
+    <row r="820" spans="1:1" ht="13.2">
       <c r="A820" s="58"/>
     </row>
-    <row r="821" spans="1:1">
+    <row r="821" spans="1:1" ht="13.2">
       <c r="A821" s="58"/>
     </row>
-    <row r="822" spans="1:1">
+    <row r="822" spans="1:1" ht="13.2">
       <c r="A822" s="58"/>
     </row>
-    <row r="823" spans="1:1">
+    <row r="823" spans="1:1" ht="13.2">
       <c r="A823" s="58"/>
     </row>
-    <row r="824" spans="1:1">
+    <row r="824" spans="1:1" ht="13.2">
       <c r="A824" s="58"/>
     </row>
-    <row r="825" spans="1:1">
+    <row r="825" spans="1:1" ht="13.2">
       <c r="A825" s="58"/>
     </row>
-    <row r="826" spans="1:1">
+    <row r="826" spans="1:1" ht="13.2">
       <c r="A826" s="58"/>
     </row>
-    <row r="827" spans="1:1">
+    <row r="827" spans="1:1" ht="13.2">
       <c r="A827" s="58"/>
     </row>
-    <row r="828" spans="1:1">
+    <row r="828" spans="1:1" ht="13.2">
       <c r="A828" s="58"/>
     </row>
-    <row r="829" spans="1:1">
+    <row r="829" spans="1:1" ht="13.2">
       <c r="A829" s="58"/>
     </row>
-    <row r="830" spans="1:1">
+    <row r="830" spans="1:1" ht="13.2">
       <c r="A830" s="58"/>
     </row>
-    <row r="831" spans="1:1">
+    <row r="831" spans="1:1" ht="13.2">
       <c r="A831" s="58"/>
     </row>
-    <row r="832" spans="1:1">
+    <row r="832" spans="1:1" ht="13.2">
       <c r="A832" s="58"/>
     </row>
-    <row r="833" spans="1:1">
+    <row r="833" spans="1:1" ht="13.2">
       <c r="A833" s="58"/>
     </row>
-    <row r="834" spans="1:1">
+    <row r="834" spans="1:1" ht="13.2">
       <c r="A834" s="58"/>
     </row>
-    <row r="835" spans="1:1">
+    <row r="835" spans="1:1" ht="13.2">
       <c r="A835" s="58"/>
     </row>
-    <row r="836" spans="1:1">
+    <row r="836" spans="1:1" ht="13.2">
       <c r="A836" s="58"/>
     </row>
-    <row r="837" spans="1:1">
+    <row r="837" spans="1:1" ht="13.2">
       <c r="A837" s="58"/>
     </row>
-    <row r="838" spans="1:1">
+    <row r="838" spans="1:1" ht="13.2">
       <c r="A838" s="58"/>
     </row>
-    <row r="839" spans="1:1">
+    <row r="839" spans="1:1" ht="13.2">
       <c r="A839" s="58"/>
     </row>
-    <row r="840" spans="1:1">
+    <row r="840" spans="1:1" ht="13.2">
       <c r="A840" s="58"/>
     </row>
-    <row r="841" spans="1:1">
+    <row r="841" spans="1:1" ht="13.2">
       <c r="A841" s="58"/>
     </row>
-    <row r="842" spans="1:1">
+    <row r="842" spans="1:1" ht="13.2">
       <c r="A842" s="58"/>
     </row>
-    <row r="843" spans="1:1">
+    <row r="843" spans="1:1" ht="13.2">
       <c r="A843" s="58"/>
     </row>
-    <row r="844" spans="1:1">
+    <row r="844" spans="1:1" ht="13.2">
       <c r="A844" s="58"/>
     </row>
-    <row r="845" spans="1:1">
+    <row r="845" spans="1:1" ht="13.2">
       <c r="A845" s="58"/>
     </row>
-    <row r="846" spans="1:1">
+    <row r="846" spans="1:1" ht="13.2">
       <c r="A846" s="58"/>
     </row>
-    <row r="847" spans="1:1">
+    <row r="847" spans="1:1" ht="13.2">
       <c r="A847" s="58"/>
     </row>
-    <row r="848" spans="1:1">
+    <row r="848" spans="1:1" ht="13.2">
       <c r="A848" s="58"/>
     </row>
-    <row r="849" spans="1:1">
+    <row r="849" spans="1:1" ht="13.2">
       <c r="A849" s="58"/>
     </row>
-    <row r="850" spans="1:1">
+    <row r="850" spans="1:1" ht="13.2">
       <c r="A850" s="58"/>
     </row>
-    <row r="851" spans="1:1">
+    <row r="851" spans="1:1" ht="13.2">
       <c r="A851" s="58"/>
     </row>
-    <row r="852" spans="1:1">
+    <row r="852" spans="1:1" ht="13.2">
       <c r="A852" s="58"/>
     </row>
-    <row r="853" spans="1:1">
+    <row r="853" spans="1:1" ht="13.2">
       <c r="A853" s="58"/>
     </row>
-    <row r="854" spans="1:1">
+    <row r="854" spans="1:1" ht="13.2">
       <c r="A854" s="58"/>
     </row>
-    <row r="855" spans="1:1">
+    <row r="855" spans="1:1" ht="13.2">
       <c r="A855" s="58"/>
     </row>
-    <row r="856" spans="1:1">
+    <row r="856" spans="1:1" ht="13.2">
       <c r="A856" s="58"/>
     </row>
-    <row r="857" spans="1:1">
+    <row r="857" spans="1:1" ht="13.2">
       <c r="A857" s="58"/>
     </row>
-    <row r="858" spans="1:1">
+    <row r="858" spans="1:1" ht="13.2">
       <c r="A858" s="58"/>
     </row>
-    <row r="859" spans="1:1">
+    <row r="859" spans="1:1" ht="13.2">
       <c r="A859" s="58"/>
     </row>
-    <row r="860" spans="1:1">
+    <row r="860" spans="1:1" ht="13.2">
       <c r="A860" s="58"/>
     </row>
-    <row r="861" spans="1:1">
+    <row r="861" spans="1:1" ht="13.2">
       <c r="A861" s="58"/>
     </row>
-    <row r="862" spans="1:1">
+    <row r="862" spans="1:1" ht="13.2">
       <c r="A862" s="58"/>
     </row>
-    <row r="863" spans="1:1">
+    <row r="863" spans="1:1" ht="13.2">
       <c r="A863" s="58"/>
     </row>
-    <row r="864" spans="1:1">
+    <row r="864" spans="1:1" ht="13.2">
       <c r="A864" s="58"/>
     </row>
-    <row r="865" spans="1:1">
+    <row r="865" spans="1:1" ht="13.2">
       <c r="A865" s="58"/>
     </row>
-    <row r="866" spans="1:1">
+    <row r="866" spans="1:1" ht="13.2">
       <c r="A866" s="58"/>
     </row>
-    <row r="867" spans="1:1">
+    <row r="867" spans="1:1" ht="13.2">
       <c r="A867" s="58"/>
     </row>
-    <row r="868" spans="1:1">
+    <row r="868" spans="1:1" ht="13.2">
       <c r="A868" s="58"/>
     </row>
-    <row r="869" spans="1:1">
+    <row r="869" spans="1:1" ht="13.2">
       <c r="A869" s="58"/>
     </row>
-    <row r="870" spans="1:1">
+    <row r="870" spans="1:1" ht="13.2">
       <c r="A870" s="58"/>
     </row>
-    <row r="871" spans="1:1">
+    <row r="871" spans="1:1" ht="13.2">
       <c r="A871" s="58"/>
     </row>
-    <row r="872" spans="1:1">
+    <row r="872" spans="1:1" ht="13.2">
       <c r="A872" s="58"/>
     </row>
-    <row r="873" spans="1:1">
+    <row r="873" spans="1:1" ht="13.2">
       <c r="A873" s="58"/>
     </row>
-    <row r="874" spans="1:1">
+    <row r="874" spans="1:1" ht="13.2">
       <c r="A874" s="58"/>
     </row>
-    <row r="875" spans="1:1">
+    <row r="875" spans="1:1" ht="13.2">
       <c r="A875" s="58"/>
     </row>
-    <row r="876" spans="1:1">
+    <row r="876" spans="1:1" ht="13.2">
       <c r="A876" s="58"/>
     </row>
-    <row r="877" spans="1:1">
+    <row r="877" spans="1:1" ht="13.2">
       <c r="A877" s="58"/>
     </row>
-    <row r="878" spans="1:1">
+    <row r="878" spans="1:1" ht="13.2">
       <c r="A878" s="58"/>
     </row>
-    <row r="879" spans="1:1">
+    <row r="879" spans="1:1" ht="13.2">
       <c r="A879" s="58"/>
     </row>
-    <row r="880" spans="1:1">
+    <row r="880" spans="1:1" ht="13.2">
       <c r="A880" s="58"/>
     </row>
-    <row r="881" spans="1:1">
+    <row r="881" spans="1:1" ht="13.2">
       <c r="A881" s="58"/>
     </row>
-    <row r="882" spans="1:1">
+    <row r="882" spans="1:1" ht="13.2">
       <c r="A882" s="58"/>
     </row>
-    <row r="883" spans="1:1">
+    <row r="883" spans="1:1" ht="13.2">
       <c r="A883" s="58"/>
     </row>
-    <row r="884" spans="1:1">
+    <row r="884" spans="1:1" ht="13.2">
       <c r="A884" s="58"/>
     </row>
-    <row r="885" spans="1:1">
+    <row r="885" spans="1:1" ht="13.2">
       <c r="A885" s="58"/>
     </row>
-    <row r="886" spans="1:1">
+    <row r="886" spans="1:1" ht="13.2">
       <c r="A886" s="58"/>
     </row>
-    <row r="887" spans="1:1">
+    <row r="887" spans="1:1" ht="13.2">
       <c r="A887" s="58"/>
     </row>
-    <row r="888" spans="1:1">
+    <row r="888" spans="1:1" ht="13.2">
       <c r="A888" s="58"/>
     </row>
-    <row r="889" spans="1:1">
+    <row r="889" spans="1:1" ht="13.2">
       <c r="A889" s="58"/>
     </row>
-    <row r="890" spans="1:1">
+    <row r="890" spans="1:1" ht="13.2">
       <c r="A890" s="58"/>
     </row>
-    <row r="891" spans="1:1">
+    <row r="891" spans="1:1" ht="13.2">
       <c r="A891" s="58"/>
     </row>
-    <row r="892" spans="1:1">
+    <row r="892" spans="1:1" ht="13.2">
       <c r="A892" s="58"/>
     </row>
-    <row r="893" spans="1:1">
+    <row r="893" spans="1:1" ht="13.2">
       <c r="A893" s="58"/>
     </row>
-    <row r="894" spans="1:1">
+    <row r="894" spans="1:1" ht="13.2">
       <c r="A894" s="58"/>
     </row>
-    <row r="895" spans="1:1">
+    <row r="895" spans="1:1" ht="13.2">
       <c r="A895" s="58"/>
     </row>
-    <row r="896" spans="1:1">
+    <row r="896" spans="1:1" ht="13.2">
       <c r="A896" s="58"/>
     </row>
-    <row r="897" spans="1:1">
+    <row r="897" spans="1:1" ht="13.2">
       <c r="A897" s="58"/>
     </row>
-    <row r="898" spans="1:1">
+    <row r="898" spans="1:1" ht="13.2">
       <c r="A898" s="58"/>
     </row>
-    <row r="899" spans="1:1">
+    <row r="899" spans="1:1" ht="13.2">
       <c r="A899" s="58"/>
     </row>
-    <row r="900" spans="1:1">
+    <row r="900" spans="1:1" ht="13.2">
       <c r="A900" s="58"/>
     </row>
-    <row r="901" spans="1:1">
+    <row r="901" spans="1:1" ht="13.2">
       <c r="A901" s="58"/>
     </row>
-    <row r="902" spans="1:1">
+    <row r="902" spans="1:1" ht="13.2">
       <c r="A902" s="58"/>
     </row>
-    <row r="903" spans="1:1">
+    <row r="903" spans="1:1" ht="13.2">
       <c r="A903" s="58"/>
     </row>
-    <row r="904" spans="1:1">
+    <row r="904" spans="1:1" ht="13.2">
       <c r="A904" s="58"/>
     </row>
-    <row r="905" spans="1:1">
+    <row r="905" spans="1:1" ht="13.2">
       <c r="A905" s="58"/>
     </row>
-    <row r="906" spans="1:1">
+    <row r="906" spans="1:1" ht="13.2">
       <c r="A906" s="58"/>
     </row>
-    <row r="907" spans="1:1">
+    <row r="907" spans="1:1" ht="13.2">
       <c r="A907" s="58"/>
     </row>
-    <row r="908" spans="1:1">
+    <row r="908" spans="1:1" ht="13.2">
       <c r="A908" s="58"/>
     </row>
-    <row r="909" spans="1:1">
+    <row r="909" spans="1:1" ht="13.2">
       <c r="A909" s="58"/>
     </row>
-    <row r="910" spans="1:1">
+    <row r="910" spans="1:1" ht="13.2">
       <c r="A910" s="58"/>
     </row>
-    <row r="911" spans="1:1">
+    <row r="911" spans="1:1" ht="13.2">
       <c r="A911" s="58"/>
     </row>
-    <row r="912" spans="1:1">
+    <row r="912" spans="1:1" ht="13.2">
       <c r="A912" s="58"/>
     </row>
-    <row r="913" spans="1:1">
+    <row r="913" spans="1:1" ht="13.2">
       <c r="A913" s="58"/>
     </row>
-    <row r="914" spans="1:1">
+    <row r="914" spans="1:1" ht="13.2">
       <c r="A914" s="58"/>
     </row>
-    <row r="915" spans="1:1">
+    <row r="915" spans="1:1" ht="13.2">
       <c r="A915" s="58"/>
     </row>
-    <row r="916" spans="1:1">
+    <row r="916" spans="1:1" ht="13.2">
       <c r="A916" s="58"/>
     </row>
-    <row r="917" spans="1:1">
+    <row r="917" spans="1:1" ht="13.2">
       <c r="A917" s="58"/>
     </row>
-    <row r="918" spans="1:1">
+    <row r="918" spans="1:1" ht="13.2">
       <c r="A918" s="58"/>
     </row>
-    <row r="919" spans="1:1">
+    <row r="919" spans="1:1" ht="13.2">
       <c r="A919" s="58"/>
     </row>
-    <row r="920" spans="1:1">
+    <row r="920" spans="1:1" ht="13.2">
       <c r="A920" s="58"/>
     </row>
-    <row r="921" spans="1:1">
+    <row r="921" spans="1:1" ht="13.2">
       <c r="A921" s="58"/>
     </row>
-    <row r="922" spans="1:1">
+    <row r="922" spans="1:1" ht="13.2">
       <c r="A922" s="58"/>
     </row>
-    <row r="923" spans="1:1">
+    <row r="923" spans="1:1" ht="13.2">
       <c r="A923" s="58"/>
     </row>
-    <row r="924" spans="1:1">
+    <row r="924" spans="1:1" ht="13.2">
       <c r="A924" s="58"/>
     </row>
-    <row r="925" spans="1:1">
+    <row r="925" spans="1:1" ht="13.2">
       <c r="A925" s="58"/>
     </row>
-    <row r="926" spans="1:1">
+    <row r="926" spans="1:1" ht="13.2">
       <c r="A926" s="58"/>
     </row>
-    <row r="927" spans="1:1">
+    <row r="927" spans="1:1" ht="13.2">
       <c r="A927" s="58"/>
     </row>
-    <row r="928" spans="1:1">
+    <row r="928" spans="1:1" ht="13.2">
       <c r="A928" s="58"/>
     </row>
-    <row r="929" spans="1:1">
+    <row r="929" spans="1:1" ht="13.2">
       <c r="A929" s="58"/>
     </row>
-    <row r="930" spans="1:1">
+    <row r="930" spans="1:1" ht="13.2">
       <c r="A930" s="58"/>
     </row>
-    <row r="931" spans="1:1">
+    <row r="931" spans="1:1" ht="13.2">
       <c r="A931" s="58"/>
     </row>
-    <row r="932" spans="1:1">
+    <row r="932" spans="1:1" ht="13.2">
       <c r="A932" s="58"/>
     </row>
-    <row r="933" spans="1:1">
+    <row r="933" spans="1:1" ht="13.2">
       <c r="A933" s="58"/>
     </row>
-    <row r="934" spans="1:1">
+    <row r="934" spans="1:1" ht="13.2">
       <c r="A934" s="58"/>
     </row>
-    <row r="935" spans="1:1">
+    <row r="935" spans="1:1" ht="13.2">
       <c r="A935" s="58"/>
     </row>
-    <row r="936" spans="1:1">
+    <row r="936" spans="1:1" ht="13.2">
       <c r="A936" s="58"/>
     </row>
-    <row r="937" spans="1:1">
+    <row r="937" spans="1:1" ht="13.2">
       <c r="A937" s="58"/>
     </row>
-    <row r="938" spans="1:1">
+    <row r="938" spans="1:1" ht="13.2">
       <c r="A938" s="58"/>
     </row>
-    <row r="939" spans="1:1">
+    <row r="939" spans="1:1" ht="13.2">
       <c r="A939" s="58"/>
     </row>
-    <row r="940" spans="1:1">
+    <row r="940" spans="1:1" ht="13.2">
       <c r="A940" s="58"/>
     </row>
-    <row r="941" spans="1:1">
+    <row r="941" spans="1:1" ht="13.2">
       <c r="A941" s="58"/>
     </row>
-    <row r="942" spans="1:1">
+    <row r="942" spans="1:1" ht="13.2">
       <c r="A942" s="58"/>
     </row>
-    <row r="943" spans="1:1">
+    <row r="943" spans="1:1" ht="13.2">
       <c r="A943" s="58"/>
     </row>
-    <row r="944" spans="1:1">
+    <row r="944" spans="1:1" ht="13.2">
       <c r="A944" s="58"/>
     </row>
-    <row r="945" spans="1:1">
+    <row r="945" spans="1:1" ht="13.2">
       <c r="A945" s="58"/>
     </row>
-    <row r="946" spans="1:1">
+    <row r="946" spans="1:1" ht="13.2">
       <c r="A946" s="58"/>
     </row>
-    <row r="947" spans="1:1">
+    <row r="947" spans="1:1" ht="13.2">
       <c r="A947" s="58"/>
     </row>
-    <row r="948" spans="1:1">
+    <row r="948" spans="1:1" ht="13.2">
       <c r="A948" s="58"/>
     </row>
-    <row r="949" spans="1:1">
+    <row r="949" spans="1:1" ht="13.2">
       <c r="A949" s="58"/>
     </row>
-    <row r="950" spans="1:1">
+    <row r="950" spans="1:1" ht="13.2">
       <c r="A950" s="58"/>
     </row>
-    <row r="951" spans="1:1">
+    <row r="951" spans="1:1" ht="13.2">
       <c r="A951" s="58"/>
     </row>
-    <row r="952" spans="1:1">
+    <row r="952" spans="1:1" ht="13.2">
       <c r="A952" s="58"/>
     </row>
-    <row r="953" spans="1:1">
+    <row r="953" spans="1:1" ht="13.2">
       <c r="A953" s="58"/>
     </row>
-    <row r="954" spans="1:1">
+    <row r="954" spans="1:1" ht="13.2">
       <c r="A954" s="58"/>
     </row>
-    <row r="955" spans="1:1">
+    <row r="955" spans="1:1" ht="13.2">
       <c r="A955" s="58"/>
     </row>
-    <row r="956" spans="1:1">
+    <row r="956" spans="1:1" ht="13.2">
       <c r="A956" s="58"/>
     </row>
-    <row r="957" spans="1:1">
+    <row r="957" spans="1:1" ht="13.2">
       <c r="A957" s="58"/>
     </row>
-    <row r="958" spans="1:1">
+    <row r="958" spans="1:1" ht="13.2">
       <c r="A958" s="58"/>
     </row>
-    <row r="959" spans="1:1">
+    <row r="959" spans="1:1" ht="13.2">
       <c r="A959" s="58"/>
     </row>
-    <row r="960" spans="1:1">
+    <row r="960" spans="1:1" ht="13.2">
       <c r="A960" s="58"/>
     </row>
-    <row r="961" spans="1:1">
+    <row r="961" spans="1:1" ht="13.2">
       <c r="A961" s="58"/>
     </row>
-    <row r="962" spans="1:1">
+    <row r="962" spans="1:1" ht="13.2">
       <c r="A962" s="58"/>
     </row>
-    <row r="963" spans="1:1">
+    <row r="963" spans="1:1" ht="13.2">
       <c r="A963" s="58"/>
     </row>
-    <row r="964" spans="1:1">
+    <row r="964" spans="1:1" ht="13.2">
       <c r="A964" s="58"/>
     </row>
-    <row r="965" spans="1:1">
+    <row r="965" spans="1:1" ht="13.2">
       <c r="A965" s="58"/>
     </row>
-    <row r="966" spans="1:1">
+    <row r="966" spans="1:1" ht="13.2">
       <c r="A966" s="58"/>
     </row>
-    <row r="967" spans="1:1">
+    <row r="967" spans="1:1" ht="13.2">
       <c r="A967" s="58"/>
     </row>
-    <row r="968" spans="1:1">
+    <row r="968" spans="1:1" ht="13.2">
       <c r="A968" s="58"/>
     </row>
-    <row r="969" spans="1:1">
+    <row r="969" spans="1:1" ht="13.2">
       <c r="A969" s="58"/>
     </row>
-    <row r="970" spans="1:1">
+    <row r="970" spans="1:1" ht="13.2">
       <c r="A970" s="58"/>
     </row>
-    <row r="971" spans="1:1">
+    <row r="971" spans="1:1" ht="13.2">
       <c r="A971" s="58"/>
     </row>
-    <row r="972" spans="1:1">
+    <row r="972" spans="1:1" ht="13.2">
       <c r="A972" s="58"/>
     </row>
-    <row r="973" spans="1:1">
+    <row r="973" spans="1:1" ht="13.2">
       <c r="A973" s="58"/>
     </row>
-    <row r="974" spans="1:1">
+    <row r="974" spans="1:1" ht="13.2">
       <c r="A974" s="58"/>
     </row>
-    <row r="975" spans="1:1">
+    <row r="975" spans="1:1" ht="13.2">
       <c r="A975" s="58"/>
     </row>
-    <row r="976" spans="1:1">
+    <row r="976" spans="1:1" ht="13.2">
       <c r="A976" s="58"/>
     </row>
-    <row r="977" spans="1:1">
+    <row r="977" spans="1:1" ht="13.2">
       <c r="A977" s="58"/>
     </row>
-    <row r="978" spans="1:1">
+    <row r="978" spans="1:1" ht="13.2">
       <c r="A978" s="58"/>
     </row>
-    <row r="979" spans="1:1">
+    <row r="979" spans="1:1" ht="13.2">
       <c r="A979" s="58"/>
     </row>
-    <row r="980" spans="1:1">
+    <row r="980" spans="1:1" ht="13.2">
       <c r="A980" s="58"/>
     </row>
-    <row r="981" spans="1:1">
+    <row r="981" spans="1:1" ht="13.2">
       <c r="A981" s="58"/>
     </row>
-    <row r="982" spans="1:1">
+    <row r="982" spans="1:1" ht="13.2">
       <c r="A982" s="58"/>
     </row>
-    <row r="983" spans="1:1">
+    <row r="983" spans="1:1" ht="13.2">
       <c r="A983" s="58"/>
     </row>
-    <row r="984" spans="1:1">
+    <row r="984" spans="1:1" ht="13.2">
       <c r="A984" s="58"/>
     </row>
-    <row r="985" spans="1:1">
+    <row r="985" spans="1:1" ht="13.2">
       <c r="A985" s="58"/>
     </row>
-    <row r="986" spans="1:1">
+    <row r="986" spans="1:1" ht="13.2">
       <c r="A986" s="58"/>
     </row>
-    <row r="987" spans="1:1">
+    <row r="987" spans="1:1" ht="13.2">
       <c r="A987" s="58"/>
     </row>
-    <row r="988" spans="1:1">
+    <row r="988" spans="1:1" ht="13.2">
       <c r="A988" s="58"/>
     </row>
-    <row r="989" spans="1:1">
+    <row r="989" spans="1:1" ht="13.2">
       <c r="A989" s="58"/>
     </row>
-    <row r="990" spans="1:1">
+    <row r="990" spans="1:1" ht="13.2">
       <c r="A990" s="58"/>
     </row>
-    <row r="991" spans="1:1">
+    <row r="991" spans="1:1" ht="13.2">
       <c r="A991" s="58"/>
     </row>
-    <row r="992" spans="1:1">
+    <row r="992" spans="1:1" ht="13.2">
       <c r="A992" s="58"/>
     </row>
-    <row r="993" spans="1:1">
+    <row r="993" spans="1:1" ht="13.2">
       <c r="A993" s="58"/>
     </row>
-    <row r="994" spans="1:1">
+    <row r="994" spans="1:1" ht="13.2">
       <c r="A994" s="58"/>
     </row>
-    <row r="995" spans="1:1">
+    <row r="995" spans="1:1" ht="13.2">
       <c r="A995" s="58"/>
     </row>
-    <row r="996" spans="1:1">
+    <row r="996" spans="1:1" ht="13.2">
       <c r="A996" s="58"/>
     </row>
-    <row r="997" spans="1:1">
+    <row r="997" spans="1:1" ht="13.2">
       <c r="A997" s="58"/>
     </row>
-    <row r="998" spans="1:1">
+    <row r="998" spans="1:1" ht="13.2">
       <c r="A998" s="58"/>
     </row>
-    <row r="999" spans="1:1">
+    <row r="999" spans="1:1" ht="13.2">
       <c r="A999" s="58"/>
     </row>
-    <row r="1000" spans="1:1">
+    <row r="1000" spans="1:1" ht="13.2">
       <c r="A1000" s="58"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" display="https://world-sailing-api.soticcloud.net/stats/api/event/b04bd77a-378c-4737-85c6-3a740b95cdcb?include=crews.country%2Ccrews.sailors.crewRole%2Craces.raceResults.crew.country%2Craces.raceResults.crew.sailors%2Craces.raceResults.crewCompetingStatus%2Craces.status%2Ccrews.carriedWins" xr:uid="{A2DEA339-F1C4-43FA-8FE4-7A699EBF031D}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>